<commit_message>
Updated the test data and set to Not Started
</commit_message>
<xml_diff>
--- a/SampleTestData.xlsx
+++ b/SampleTestData.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john.lester.f.lucena\Desktop\hcm_new_configuration\HCM_Configurations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo.t.lambojon\Desktop\secret\HCM-Configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -142,22 +142,22 @@
     <t>ConfigureOfferingsTest</t>
   </si>
   <si>
+    <t>Test Case 2</t>
+  </si>
+  <si>
+    <t>Customer Data Management</t>
+  </si>
+  <si>
+    <t>Data Quality</t>
+  </si>
+  <si>
+    <t>Customer Data Management Business Intelligence Analytics</t>
+  </si>
+  <si>
+    <t>Customer Hub</t>
+  </si>
+  <si>
     <t>Not Started</t>
-  </si>
-  <si>
-    <t>Test Case 2</t>
-  </si>
-  <si>
-    <t>Customer Data Management</t>
-  </si>
-  <si>
-    <t>Data Quality</t>
-  </si>
-  <si>
-    <t>Customer Data Management Business Intelligence Analytics</t>
-  </si>
-  <si>
-    <t>Customer Hub</t>
   </si>
 </sst>
 </file>
@@ -861,6 +861,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:FU3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1775,6 +1776,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:FU3"/>
   <sheetViews>
     <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
@@ -2645,11 +2647,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:FY4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3346,25 +3349,25 @@
         <v>33</v>
       </c>
       <c r="J3" s="25" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="K3" s="21" t="s">
         <v>34</v>
       </c>
       <c r="L3" s="25" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="M3" s="32" t="s">
         <v>36</v>
       </c>
       <c r="N3" s="25" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="O3" s="28" t="s">
         <v>35</v>
       </c>
       <c r="P3" s="25" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="Q3" s="26"/>
       <c r="R3" s="16"/>
@@ -3534,7 +3537,7 @@
     </row>
     <row r="4" spans="1:181" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>37</v>
@@ -3553,30 +3556,35 @@
         <v>11</v>
       </c>
       <c r="H4" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="J4" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="21" t="s">
+      <c r="L4" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="L4" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="M4" s="32" t="s">
+      <c r="N4" s="25" t="s">
         <v>43</v>
-      </c>
-      <c r="N4" s="25" t="s">
-        <v>38</v>
       </c>
       <c r="O4" s="28"/>
       <c r="P4" s="25"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J4 L3:L4 N3:N4 P3">
+      <formula1>"Not Started,In Progress,Implemented"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1"/>
     <hyperlink ref="E4" r:id="rId2"/>

</xml_diff>

<commit_message>
Updated 18 configurations with Dropdown box
</commit_message>
<xml_diff>
--- a/SampleTestData.xlsx
+++ b/SampleTestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo.t.lambojon\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo.t.lambojon\Desktop\secret\paoloxide\project-repo\paoloxide-HCM_Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Manage Performance" sheetId="7" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="205">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -498,6 +498,150 @@
   </si>
   <si>
     <t>Advanced Catalogs</t>
+  </si>
+  <si>
+    <t>Test Case 14</t>
+  </si>
+  <si>
+    <t>Project Financial Management</t>
+  </si>
+  <si>
+    <t>Burdening</t>
+  </si>
+  <si>
+    <t>Project Control</t>
+  </si>
+  <si>
+    <t>Project Costing</t>
+  </si>
+  <si>
+    <t>Project Billing</t>
+  </si>
+  <si>
+    <t>Project Business Intelligence Analytics</t>
+  </si>
+  <si>
+    <t>Project Revenue and Billing Business Intelligence Analytics</t>
+  </si>
+  <si>
+    <t>Project Performance Business Intelligence Analytics</t>
+  </si>
+  <si>
+    <t>Project Control and Costing Business Intelligence Analytics</t>
+  </si>
+  <si>
+    <t>Risk and Controls</t>
+  </si>
+  <si>
+    <t>Test Case 15</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Sales Prediction Engine</t>
+  </si>
+  <si>
+    <t>Outlook Integration</t>
+  </si>
+  <si>
+    <t>Quotas</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>Competitors</t>
+  </si>
+  <si>
+    <t>Sales Forecasting</t>
+  </si>
+  <si>
+    <t>Partners</t>
+  </si>
+  <si>
+    <t>Partner Business Intelligence Analytics</t>
+  </si>
+  <si>
+    <t>Partner Performance</t>
+  </si>
+  <si>
+    <t>Partner Deals</t>
+  </si>
+  <si>
+    <t>Partner Programs</t>
+  </si>
+  <si>
+    <t>Territory Management</t>
+  </si>
+  <si>
+    <t>Sales Business Intelligence Analytics</t>
+  </si>
+  <si>
+    <t>Quota Management Business Intelligence Analytics</t>
+  </si>
+  <si>
+    <t>Territory Management Business Intelligence Analytics</t>
+  </si>
+  <si>
+    <t>Opportunity and Revenue Management Business Intelligence Analytics</t>
+  </si>
+  <si>
+    <t>Customer Interactions Management</t>
+  </si>
+  <si>
+    <t>Sales Forecasting Management Business Intelligence Analytics</t>
+  </si>
+  <si>
+    <t>Basic Catalogs</t>
+  </si>
+  <si>
+    <t>Sales Cloud Integration</t>
+  </si>
+  <si>
+    <t>Test Case 16</t>
+  </si>
+  <si>
+    <t>Supply Chain Financial Orchestration</t>
+  </si>
+  <si>
+    <t>Test Case 17</t>
+  </si>
+  <si>
+    <t>Supply Chain Managerial Accounting</t>
+  </si>
+  <si>
+    <t>Receipt Accounting</t>
+  </si>
+  <si>
+    <t>Cost Accounting</t>
+  </si>
+  <si>
+    <t>Cost and Profit Planning</t>
+  </si>
+  <si>
+    <t>Test Case 18</t>
+  </si>
+  <si>
+    <t>Payroll</t>
+  </si>
+  <si>
+    <t>Workforce Scheduling</t>
+  </si>
+  <si>
+    <t>Workforce Predictions</t>
+  </si>
+  <si>
+    <t>Time and Labor</t>
+  </si>
+  <si>
+    <t>Network at Work</t>
+  </si>
+  <si>
+    <t>Workforce Management</t>
+  </si>
+  <si>
+    <t>Test Case 13</t>
   </si>
 </sst>
 </file>
@@ -673,7 +817,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -735,13 +879,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -769,6 +906,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2838,22 +2978,22 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:EW14"/>
+  <dimension ref="A1:EW20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J30" sqref="J30"/>
+      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="30" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="76.85546875" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="17" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" customWidth="1"/>
+    <col min="5" max="5" width="76.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="67.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.5703125" customWidth="1"/>
@@ -2873,39 +3013,39 @@
     <col min="24" max="24" width="18.85546875" customWidth="1"/>
     <col min="25" max="25" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="20.42578125" customWidth="1"/>
-    <col min="27" max="27" width="42" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="54.85546875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="12.28515625" customWidth="1"/>
-    <col min="29" max="29" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="58.140625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="19.42578125" customWidth="1"/>
-    <col min="31" max="31" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="51.42578125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="19.85546875" customWidth="1"/>
-    <col min="33" max="33" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="57.85546875" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="12.28515625" customWidth="1"/>
     <col min="35" max="35" width="50.7109375" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="18.85546875" customWidth="1"/>
-    <col min="37" max="37" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="52.5703125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17.42578125" customWidth="1"/>
-    <col min="39" max="39" width="8.7109375" customWidth="1"/>
+    <col min="39" max="39" width="69.7109375" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="12.28515625" customWidth="1"/>
-    <col min="41" max="41" width="16.85546875" customWidth="1"/>
+    <col min="41" max="41" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="19.140625" customWidth="1"/>
-    <col min="43" max="43" width="11.5703125" customWidth="1"/>
+    <col min="43" max="43" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="19.140625" customWidth="1"/>
-    <col min="45" max="45" width="8.7109375" customWidth="1"/>
+    <col min="45" max="45" width="54.42578125" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="12.28515625" customWidth="1"/>
-    <col min="47" max="47" width="14.28515625" customWidth="1"/>
+    <col min="47" max="47" width="54.42578125" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="16.85546875" customWidth="1"/>
-    <col min="49" max="49" width="18.85546875" customWidth="1"/>
+    <col min="49" max="49" width="62.42578125" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="11.5703125" customWidth="1"/>
     <col min="51" max="51" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="8.7109375" customWidth="1"/>
+    <col min="52" max="52" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="14.28515625" customWidth="1"/>
-    <col min="55" max="55" width="48.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="48.7109375" style="21" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="30" style="24" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="30" style="21" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="37.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="37.28515625" style="21" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="48.85546875" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -3206,7 +3346,7 @@
       <c r="EM1" s="1"/>
       <c r="EN1" s="1"/>
     </row>
-    <row r="2" spans="1:153" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:153" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -3256,7 +3396,7 @@
         <v>27</v>
       </c>
       <c r="Q2" s="8"/>
-      <c r="R2" s="21"/>
+      <c r="R2" s="8"/>
       <c r="S2" s="8"/>
       <c r="T2" s="8"/>
       <c r="U2" s="8"/>
@@ -3404,7 +3544,7 @@
       <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="31" t="s">
         <v>31</v>
       </c>
       <c r="F3" s="12" t="s">
@@ -3603,7 +3743,7 @@
       <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="31" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="12" t="s">
@@ -3645,52 +3785,52 @@
       <c r="R4" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="S4" s="23"/>
+      <c r="S4" s="14"/>
       <c r="T4" s="14"/>
-      <c r="U4" s="23"/>
+      <c r="U4" s="14"/>
       <c r="V4" s="14"/>
-      <c r="W4" s="23"/>
+      <c r="W4" s="14"/>
       <c r="X4" s="14"/>
-      <c r="Y4" s="23"/>
+      <c r="Y4" s="14"/>
       <c r="Z4" s="14"/>
-      <c r="AA4" s="23"/>
+      <c r="AA4" s="14"/>
       <c r="AB4" s="14"/>
-      <c r="AC4" s="23"/>
+      <c r="AC4" s="14"/>
       <c r="AD4" s="14"/>
-      <c r="AE4" s="23"/>
+      <c r="AE4" s="14"/>
       <c r="AF4" s="14"/>
-      <c r="AG4" s="23"/>
+      <c r="AG4" s="14"/>
       <c r="AH4" s="14"/>
-      <c r="AI4" s="23"/>
+      <c r="AI4" s="14"/>
       <c r="AJ4" s="14"/>
-      <c r="AK4" s="23"/>
+      <c r="AK4" s="14"/>
       <c r="AL4" s="14"/>
-      <c r="AM4" s="23"/>
-      <c r="AN4" s="23"/>
-      <c r="AO4" s="23"/>
-      <c r="AP4" s="23"/>
-      <c r="AQ4" s="23"/>
-      <c r="AR4" s="23"/>
-      <c r="AS4" s="23"/>
-      <c r="AT4" s="23"/>
-      <c r="AU4" s="23"/>
-      <c r="AV4" s="23"/>
-      <c r="AW4" s="23"/>
-      <c r="AX4" s="23"/>
-      <c r="AY4" s="23"/>
-      <c r="AZ4" s="23"/>
-      <c r="BA4" s="23"/>
-      <c r="BB4" s="23"/>
+      <c r="AM4" s="14"/>
+      <c r="AN4" s="14"/>
+      <c r="AO4" s="14"/>
+      <c r="AP4" s="14"/>
+      <c r="AQ4" s="14"/>
+      <c r="AR4" s="14"/>
+      <c r="AS4" s="14"/>
+      <c r="AT4" s="14"/>
+      <c r="AU4" s="14"/>
+      <c r="AV4" s="14"/>
+      <c r="AW4" s="14"/>
+      <c r="AX4" s="14"/>
+      <c r="AY4" s="14"/>
+      <c r="AZ4" s="14"/>
+      <c r="BA4" s="14"/>
+      <c r="BB4" s="14"/>
       <c r="BC4" s="14"/>
-      <c r="BD4" s="22"/>
+      <c r="BD4" s="14"/>
       <c r="BE4" s="14"/>
-      <c r="BF4" s="22"/>
+      <c r="BF4" s="14"/>
       <c r="BG4" s="14"/>
-      <c r="BH4" s="22"/>
-      <c r="BI4" s="22"/>
-      <c r="BJ4" s="22"/>
-      <c r="BK4" s="22"/>
-      <c r="BL4" s="22"/>
+      <c r="BH4" s="14"/>
+      <c r="BI4" s="14"/>
+      <c r="BJ4" s="14"/>
+      <c r="BK4" s="14"/>
+      <c r="BL4" s="14"/>
     </row>
     <row r="5" spans="1:153" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -3703,7 +3843,7 @@
       <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="31" t="s">
         <v>31</v>
       </c>
       <c r="F5" s="12" t="s">
@@ -3712,73 +3852,73 @@
       <c r="G5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="14" t="s">
         <v>65</v>
       </c>
       <c r="J5" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="K5" s="23" t="s">
+      <c r="K5" s="14" t="s">
         <v>66</v>
       </c>
       <c r="L5" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="M5" s="23"/>
+      <c r="M5" s="14"/>
       <c r="N5" s="14"/>
-      <c r="O5" s="23"/>
+      <c r="O5" s="14"/>
       <c r="P5" s="14"/>
-      <c r="Q5" s="23"/>
+      <c r="Q5" s="14"/>
       <c r="R5" s="14"/>
-      <c r="S5" s="23"/>
+      <c r="S5" s="14"/>
       <c r="T5" s="14"/>
-      <c r="U5" s="23"/>
+      <c r="U5" s="14"/>
       <c r="V5" s="14"/>
-      <c r="W5" s="23"/>
+      <c r="W5" s="14"/>
       <c r="X5" s="14"/>
-      <c r="Y5" s="23"/>
+      <c r="Y5" s="14"/>
       <c r="Z5" s="14"/>
-      <c r="AA5" s="23"/>
+      <c r="AA5" s="14"/>
       <c r="AB5" s="14"/>
-      <c r="AC5" s="23"/>
+      <c r="AC5" s="14"/>
       <c r="AD5" s="14"/>
-      <c r="AE5" s="23"/>
+      <c r="AE5" s="14"/>
       <c r="AF5" s="14"/>
-      <c r="AG5" s="23"/>
+      <c r="AG5" s="14"/>
       <c r="AH5" s="14"/>
-      <c r="AI5" s="23"/>
+      <c r="AI5" s="14"/>
       <c r="AJ5" s="14"/>
-      <c r="AK5" s="23"/>
+      <c r="AK5" s="14"/>
       <c r="AL5" s="14"/>
-      <c r="AM5" s="23"/>
-      <c r="AN5" s="23"/>
-      <c r="AO5" s="23"/>
-      <c r="AP5" s="23"/>
-      <c r="AQ5" s="23"/>
-      <c r="AR5" s="23"/>
-      <c r="AS5" s="23"/>
-      <c r="AT5" s="23"/>
-      <c r="AU5" s="23"/>
-      <c r="AV5" s="23"/>
-      <c r="AW5" s="23"/>
-      <c r="AX5" s="23"/>
-      <c r="AY5" s="23"/>
-      <c r="AZ5" s="23"/>
-      <c r="BA5" s="23"/>
-      <c r="BB5" s="23"/>
+      <c r="AM5" s="14"/>
+      <c r="AN5" s="14"/>
+      <c r="AO5" s="14"/>
+      <c r="AP5" s="14"/>
+      <c r="AQ5" s="14"/>
+      <c r="AR5" s="14"/>
+      <c r="AS5" s="14"/>
+      <c r="AT5" s="14"/>
+      <c r="AU5" s="14"/>
+      <c r="AV5" s="14"/>
+      <c r="AW5" s="14"/>
+      <c r="AX5" s="14"/>
+      <c r="AY5" s="14"/>
+      <c r="AZ5" s="14"/>
+      <c r="BA5" s="14"/>
+      <c r="BB5" s="14"/>
       <c r="BC5" s="14"/>
-      <c r="BD5" s="22"/>
+      <c r="BD5" s="14"/>
       <c r="BE5" s="14"/>
-      <c r="BF5" s="22"/>
+      <c r="BF5" s="14"/>
       <c r="BG5" s="14"/>
-      <c r="BH5" s="22"/>
-      <c r="BI5" s="22"/>
-      <c r="BJ5" s="22"/>
-      <c r="BK5" s="22"/>
-      <c r="BL5" s="22"/>
+      <c r="BH5" s="14"/>
+      <c r="BI5" s="14"/>
+      <c r="BJ5" s="14"/>
+      <c r="BK5" s="14"/>
+      <c r="BL5" s="14"/>
     </row>
     <row r="6" spans="1:153" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -3791,7 +3931,7 @@
       <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="31" t="s">
         <v>31</v>
       </c>
       <c r="F6" s="12" t="s">
@@ -3800,125 +3940,125 @@
       <c r="G6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="14" t="s">
         <v>68</v>
       </c>
       <c r="J6" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="K6" s="23" t="s">
+      <c r="K6" s="14" t="s">
         <v>69</v>
       </c>
       <c r="L6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="M6" s="23" t="s">
+      <c r="M6" s="14" t="s">
         <v>70</v>
       </c>
       <c r="N6" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="O6" s="23" t="s">
+      <c r="O6" s="14" t="s">
         <v>71</v>
       </c>
       <c r="P6" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="Q6" s="23" t="s">
+      <c r="Q6" s="14" t="s">
         <v>72</v>
       </c>
       <c r="R6" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="S6" s="23" t="s">
+      <c r="S6" s="14" t="s">
         <v>73</v>
       </c>
       <c r="T6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="U6" s="23" t="s">
+      <c r="U6" s="14" t="s">
         <v>74</v>
       </c>
       <c r="V6" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="W6" s="23" t="s">
+      <c r="W6" s="14" t="s">
         <v>141</v>
       </c>
       <c r="X6" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="Y6" s="23" t="s">
+      <c r="Y6" s="14" t="s">
         <v>75</v>
       </c>
       <c r="Z6" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AA6" s="23" t="s">
+      <c r="AA6" s="14" t="s">
         <v>76</v>
       </c>
       <c r="AB6" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AC6" s="23" t="s">
+      <c r="AC6" s="14" t="s">
         <v>77</v>
       </c>
       <c r="AD6" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AE6" s="23" t="s">
+      <c r="AE6" s="14" t="s">
         <v>78</v>
       </c>
       <c r="AF6" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AG6" s="23" t="s">
+      <c r="AG6" s="14" t="s">
         <v>79</v>
       </c>
       <c r="AH6" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AI6" s="23" t="s">
+      <c r="AI6" s="14" t="s">
         <v>80</v>
       </c>
       <c r="AJ6" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AK6" s="23" t="s">
+      <c r="AK6" s="14" t="s">
         <v>81</v>
       </c>
       <c r="AL6" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AM6" s="23"/>
-      <c r="AN6" s="23"/>
-      <c r="AO6" s="23"/>
-      <c r="AP6" s="23"/>
-      <c r="AQ6" s="23"/>
-      <c r="AR6" s="23"/>
-      <c r="AS6" s="23"/>
-      <c r="AT6" s="23"/>
-      <c r="AU6" s="23"/>
-      <c r="AV6" s="23"/>
-      <c r="AW6" s="23"/>
-      <c r="AX6" s="23"/>
-      <c r="AY6" s="23"/>
-      <c r="AZ6" s="23"/>
-      <c r="BA6" s="23"/>
-      <c r="BB6" s="23"/>
+      <c r="AM6" s="14"/>
+      <c r="AN6" s="14"/>
+      <c r="AO6" s="14"/>
+      <c r="AP6" s="14"/>
+      <c r="AQ6" s="14"/>
+      <c r="AR6" s="14"/>
+      <c r="AS6" s="14"/>
+      <c r="AT6" s="14"/>
+      <c r="AU6" s="14"/>
+      <c r="AV6" s="14"/>
+      <c r="AW6" s="14"/>
+      <c r="AX6" s="14"/>
+      <c r="AY6" s="14"/>
+      <c r="AZ6" s="14"/>
+      <c r="BA6" s="14"/>
+      <c r="BB6" s="14"/>
       <c r="BC6" s="14"/>
-      <c r="BD6" s="22"/>
+      <c r="BD6" s="14"/>
       <c r="BE6" s="14"/>
-      <c r="BF6" s="22"/>
+      <c r="BF6" s="14"/>
       <c r="BG6" s="14"/>
-      <c r="BH6" s="22"/>
-      <c r="BI6" s="22"/>
-      <c r="BJ6" s="22"/>
-      <c r="BK6" s="22"/>
-      <c r="BL6" s="22"/>
+      <c r="BH6" s="14"/>
+      <c r="BI6" s="14"/>
+      <c r="BJ6" s="14"/>
+      <c r="BK6" s="14"/>
+      <c r="BL6" s="14"/>
     </row>
     <row r="7" spans="1:153" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -3931,7 +4071,7 @@
       <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="31" t="s">
         <v>31</v>
       </c>
       <c r="F7" s="12" t="s">
@@ -3940,73 +4080,73 @@
       <c r="G7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="14" t="s">
         <v>133</v>
       </c>
       <c r="J7" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="K7" s="23" t="s">
+      <c r="K7" s="14" t="s">
         <v>74</v>
       </c>
       <c r="L7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="M7" s="23"/>
+      <c r="M7" s="14"/>
       <c r="N7" s="14"/>
-      <c r="O7" s="23"/>
+      <c r="O7" s="14"/>
       <c r="P7" s="14"/>
-      <c r="Q7" s="23"/>
+      <c r="Q7" s="14"/>
       <c r="R7" s="14"/>
-      <c r="S7" s="23"/>
+      <c r="S7" s="14"/>
       <c r="T7" s="14"/>
-      <c r="U7" s="23"/>
+      <c r="U7" s="14"/>
       <c r="V7" s="14"/>
-      <c r="W7" s="23"/>
+      <c r="W7" s="14"/>
       <c r="X7" s="14"/>
-      <c r="Y7" s="23"/>
+      <c r="Y7" s="14"/>
       <c r="Z7" s="14"/>
-      <c r="AA7" s="23"/>
+      <c r="AA7" s="14"/>
       <c r="AB7" s="14"/>
-      <c r="AC7" s="23"/>
+      <c r="AC7" s="14"/>
       <c r="AD7" s="14"/>
-      <c r="AE7" s="23"/>
+      <c r="AE7" s="14"/>
       <c r="AF7" s="14"/>
-      <c r="AG7" s="23"/>
+      <c r="AG7" s="14"/>
       <c r="AH7" s="14"/>
-      <c r="AI7" s="23"/>
+      <c r="AI7" s="14"/>
       <c r="AJ7" s="14"/>
-      <c r="AK7" s="23"/>
+      <c r="AK7" s="14"/>
       <c r="AL7" s="14"/>
-      <c r="AM7" s="23"/>
-      <c r="AN7" s="23"/>
-      <c r="AO7" s="23"/>
-      <c r="AP7" s="23"/>
-      <c r="AQ7" s="23"/>
-      <c r="AR7" s="23"/>
-      <c r="AS7" s="23"/>
-      <c r="AT7" s="23"/>
-      <c r="AU7" s="23"/>
-      <c r="AV7" s="23"/>
-      <c r="AW7" s="23"/>
-      <c r="AX7" s="23"/>
-      <c r="AY7" s="23"/>
-      <c r="AZ7" s="23"/>
-      <c r="BA7" s="23"/>
-      <c r="BB7" s="23"/>
+      <c r="AM7" s="14"/>
+      <c r="AN7" s="14"/>
+      <c r="AO7" s="14"/>
+      <c r="AP7" s="14"/>
+      <c r="AQ7" s="14"/>
+      <c r="AR7" s="14"/>
+      <c r="AS7" s="14"/>
+      <c r="AT7" s="14"/>
+      <c r="AU7" s="14"/>
+      <c r="AV7" s="14"/>
+      <c r="AW7" s="14"/>
+      <c r="AX7" s="14"/>
+      <c r="AY7" s="14"/>
+      <c r="AZ7" s="14"/>
+      <c r="BA7" s="14"/>
+      <c r="BB7" s="14"/>
       <c r="BC7" s="14"/>
-      <c r="BD7" s="22"/>
+      <c r="BD7" s="14"/>
       <c r="BE7" s="14"/>
-      <c r="BF7" s="22"/>
+      <c r="BF7" s="14"/>
       <c r="BG7" s="14"/>
-      <c r="BH7" s="22"/>
-      <c r="BI7" s="22"/>
-      <c r="BJ7" s="22"/>
-      <c r="BK7" s="22"/>
-      <c r="BL7" s="22"/>
+      <c r="BH7" s="14"/>
+      <c r="BI7" s="14"/>
+      <c r="BJ7" s="14"/>
+      <c r="BK7" s="14"/>
+      <c r="BL7" s="14"/>
     </row>
     <row r="8" spans="1:153" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -4019,7 +4159,7 @@
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="31" t="s">
         <v>31</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -4028,89 +4168,89 @@
       <c r="G8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="14" t="s">
         <v>84</v>
       </c>
       <c r="J8" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="23" t="s">
+      <c r="K8" s="14" t="s">
         <v>85</v>
       </c>
       <c r="L8" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="M8" s="23" t="s">
+      <c r="M8" s="14" t="s">
         <v>86</v>
       </c>
       <c r="N8" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="O8" s="23" t="s">
+      <c r="O8" s="14" t="s">
         <v>87</v>
       </c>
       <c r="P8" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="Q8" s="23" t="s">
+      <c r="Q8" s="14" t="s">
         <v>88</v>
       </c>
       <c r="R8" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="S8" s="23" t="s">
+      <c r="S8" s="14" t="s">
         <v>89</v>
       </c>
       <c r="T8" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="U8" s="23"/>
+      <c r="U8" s="14"/>
       <c r="V8" s="14"/>
-      <c r="W8" s="23"/>
+      <c r="W8" s="14"/>
       <c r="X8" s="14"/>
-      <c r="Y8" s="23"/>
+      <c r="Y8" s="14"/>
       <c r="Z8" s="14"/>
-      <c r="AA8" s="23"/>
+      <c r="AA8" s="14"/>
       <c r="AB8" s="14"/>
-      <c r="AC8" s="23"/>
+      <c r="AC8" s="14"/>
       <c r="AD8" s="14"/>
-      <c r="AE8" s="23"/>
+      <c r="AE8" s="14"/>
       <c r="AF8" s="14"/>
-      <c r="AG8" s="23"/>
+      <c r="AG8" s="14"/>
       <c r="AH8" s="14"/>
-      <c r="AI8" s="23"/>
+      <c r="AI8" s="14"/>
       <c r="AJ8" s="14"/>
-      <c r="AK8" s="23"/>
+      <c r="AK8" s="14"/>
       <c r="AL8" s="14"/>
-      <c r="AM8" s="23"/>
-      <c r="AN8" s="23"/>
-      <c r="AO8" s="23"/>
-      <c r="AP8" s="23"/>
-      <c r="AQ8" s="23"/>
-      <c r="AR8" s="23"/>
-      <c r="AS8" s="23"/>
-      <c r="AT8" s="23"/>
-      <c r="AU8" s="23"/>
-      <c r="AV8" s="23"/>
-      <c r="AW8" s="23"/>
-      <c r="AX8" s="23"/>
-      <c r="AY8" s="23"/>
-      <c r="AZ8" s="23"/>
-      <c r="BA8" s="23"/>
-      <c r="BB8" s="23"/>
+      <c r="AM8" s="14"/>
+      <c r="AN8" s="14"/>
+      <c r="AO8" s="14"/>
+      <c r="AP8" s="14"/>
+      <c r="AQ8" s="14"/>
+      <c r="AR8" s="14"/>
+      <c r="AS8" s="14"/>
+      <c r="AT8" s="14"/>
+      <c r="AU8" s="14"/>
+      <c r="AV8" s="14"/>
+      <c r="AW8" s="14"/>
+      <c r="AX8" s="14"/>
+      <c r="AY8" s="14"/>
+      <c r="AZ8" s="14"/>
+      <c r="BA8" s="14"/>
+      <c r="BB8" s="14"/>
       <c r="BC8" s="14"/>
-      <c r="BD8" s="22"/>
+      <c r="BD8" s="14"/>
       <c r="BE8" s="14"/>
-      <c r="BF8" s="22"/>
+      <c r="BF8" s="14"/>
       <c r="BG8" s="14"/>
-      <c r="BH8" s="22"/>
-      <c r="BI8" s="22"/>
-      <c r="BJ8" s="22"/>
-      <c r="BK8" s="22"/>
-      <c r="BL8" s="22"/>
+      <c r="BH8" s="14"/>
+      <c r="BI8" s="14"/>
+      <c r="BJ8" s="14"/>
+      <c r="BK8" s="14"/>
+      <c r="BL8" s="14"/>
     </row>
     <row r="9" spans="1:153" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -4123,7 +4263,7 @@
       <c r="D9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="31" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="12" t="s">
@@ -4132,67 +4272,67 @@
       <c r="G9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="14" t="s">
         <v>90</v>
       </c>
       <c r="I9" s="14" t="s">
         <v>47</v>
       </c>
       <c r="J9" s="14"/>
-      <c r="K9" s="23"/>
+      <c r="K9" s="14"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="23"/>
+      <c r="M9" s="14"/>
       <c r="N9" s="14"/>
-      <c r="O9" s="23"/>
+      <c r="O9" s="14"/>
       <c r="P9" s="14"/>
-      <c r="Q9" s="23"/>
+      <c r="Q9" s="14"/>
       <c r="R9" s="14"/>
-      <c r="S9" s="23"/>
+      <c r="S9" s="14"/>
       <c r="T9" s="14"/>
-      <c r="U9" s="23"/>
+      <c r="U9" s="14"/>
       <c r="V9" s="14"/>
-      <c r="W9" s="23"/>
+      <c r="W9" s="14"/>
       <c r="X9" s="14"/>
-      <c r="Y9" s="23"/>
+      <c r="Y9" s="14"/>
       <c r="Z9" s="14"/>
-      <c r="AA9" s="23"/>
+      <c r="AA9" s="14"/>
       <c r="AB9" s="14"/>
-      <c r="AC9" s="23"/>
+      <c r="AC9" s="14"/>
       <c r="AD9" s="14"/>
-      <c r="AE9" s="23"/>
+      <c r="AE9" s="14"/>
       <c r="AF9" s="14"/>
-      <c r="AG9" s="23"/>
+      <c r="AG9" s="14"/>
       <c r="AH9" s="14"/>
-      <c r="AI9" s="23"/>
+      <c r="AI9" s="14"/>
       <c r="AJ9" s="14"/>
-      <c r="AK9" s="23"/>
+      <c r="AK9" s="14"/>
       <c r="AL9" s="14"/>
-      <c r="AM9" s="23"/>
-      <c r="AN9" s="23"/>
-      <c r="AO9" s="23"/>
-      <c r="AP9" s="23"/>
-      <c r="AQ9" s="23"/>
-      <c r="AR9" s="23"/>
-      <c r="AS9" s="23"/>
-      <c r="AT9" s="23"/>
-      <c r="AU9" s="23"/>
-      <c r="AV9" s="23"/>
-      <c r="AW9" s="23"/>
-      <c r="AX9" s="23"/>
-      <c r="AY9" s="23"/>
-      <c r="AZ9" s="23"/>
-      <c r="BA9" s="23"/>
-      <c r="BB9" s="23"/>
+      <c r="AM9" s="14"/>
+      <c r="AN9" s="14"/>
+      <c r="AO9" s="14"/>
+      <c r="AP9" s="14"/>
+      <c r="AQ9" s="14"/>
+      <c r="AR9" s="14"/>
+      <c r="AS9" s="14"/>
+      <c r="AT9" s="14"/>
+      <c r="AU9" s="14"/>
+      <c r="AV9" s="14"/>
+      <c r="AW9" s="14"/>
+      <c r="AX9" s="14"/>
+      <c r="AY9" s="14"/>
+      <c r="AZ9" s="14"/>
+      <c r="BA9" s="14"/>
+      <c r="BB9" s="14"/>
       <c r="BC9" s="14"/>
-      <c r="BD9" s="22"/>
+      <c r="BD9" s="14"/>
       <c r="BE9" s="14"/>
-      <c r="BF9" s="22"/>
+      <c r="BF9" s="14"/>
       <c r="BG9" s="14"/>
-      <c r="BH9" s="22"/>
-      <c r="BI9" s="22"/>
-      <c r="BJ9" s="22"/>
-      <c r="BK9" s="22"/>
-      <c r="BL9" s="22"/>
+      <c r="BH9" s="14"/>
+      <c r="BI9" s="14"/>
+      <c r="BJ9" s="14"/>
+      <c r="BK9" s="14"/>
+      <c r="BL9" s="14"/>
     </row>
     <row r="10" spans="1:153" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -4205,7 +4345,7 @@
       <c r="D10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="31" t="s">
         <v>31</v>
       </c>
       <c r="F10" s="12" t="s">
@@ -4214,105 +4354,105 @@
       <c r="G10" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="H10" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="I10" s="23" t="s">
+      <c r="I10" s="14" t="s">
         <v>134</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="K10" s="23" t="s">
+      <c r="K10" s="14" t="s">
         <v>96</v>
       </c>
       <c r="L10" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="M10" s="23" t="s">
+      <c r="M10" s="14" t="s">
         <v>97</v>
       </c>
       <c r="N10" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="O10" s="23" t="s">
+      <c r="O10" s="14" t="s">
         <v>98</v>
       </c>
       <c r="P10" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="Q10" s="23" t="s">
+      <c r="Q10" s="14" t="s">
         <v>99</v>
       </c>
       <c r="R10" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="S10" s="23" t="s">
+      <c r="S10" s="14" t="s">
         <v>100</v>
       </c>
       <c r="T10" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="U10" s="23" t="s">
+      <c r="U10" s="14" t="s">
         <v>101</v>
       </c>
       <c r="V10" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="W10" s="23" t="s">
+      <c r="W10" s="14" t="s">
         <v>102</v>
       </c>
       <c r="X10" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="Y10" s="23" t="s">
+      <c r="Y10" s="14" t="s">
         <v>103</v>
       </c>
       <c r="Z10" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AA10" s="23" t="s">
+      <c r="AA10" s="14" t="s">
         <v>104</v>
       </c>
       <c r="AB10" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AC10" s="23"/>
+      <c r="AC10" s="14"/>
       <c r="AD10" s="14"/>
-      <c r="AE10" s="23"/>
+      <c r="AE10" s="14"/>
       <c r="AF10" s="14"/>
-      <c r="AG10" s="23"/>
+      <c r="AG10" s="14"/>
       <c r="AH10" s="14"/>
-      <c r="AI10" s="23"/>
+      <c r="AI10" s="14"/>
       <c r="AJ10" s="14"/>
-      <c r="AK10" s="23"/>
+      <c r="AK10" s="14"/>
       <c r="AL10" s="14"/>
-      <c r="AM10" s="23"/>
-      <c r="AN10" s="23"/>
-      <c r="AO10" s="23"/>
-      <c r="AP10" s="23"/>
-      <c r="AQ10" s="23"/>
-      <c r="AR10" s="23"/>
-      <c r="AS10" s="23"/>
-      <c r="AT10" s="23"/>
-      <c r="AU10" s="23"/>
-      <c r="AV10" s="23"/>
-      <c r="AW10" s="23"/>
-      <c r="AX10" s="23"/>
-      <c r="AY10" s="23"/>
-      <c r="AZ10" s="23"/>
-      <c r="BA10" s="23"/>
-      <c r="BB10" s="23"/>
+      <c r="AM10" s="14"/>
+      <c r="AN10" s="14"/>
+      <c r="AO10" s="14"/>
+      <c r="AP10" s="14"/>
+      <c r="AQ10" s="14"/>
+      <c r="AR10" s="14"/>
+      <c r="AS10" s="14"/>
+      <c r="AT10" s="14"/>
+      <c r="AU10" s="14"/>
+      <c r="AV10" s="14"/>
+      <c r="AW10" s="14"/>
+      <c r="AX10" s="14"/>
+      <c r="AY10" s="14"/>
+      <c r="AZ10" s="14"/>
+      <c r="BA10" s="14"/>
+      <c r="BB10" s="14"/>
       <c r="BC10" s="14"/>
-      <c r="BD10" s="22"/>
+      <c r="BD10" s="14"/>
       <c r="BE10" s="14"/>
-      <c r="BF10" s="22"/>
+      <c r="BF10" s="14"/>
       <c r="BG10" s="14"/>
-      <c r="BH10" s="22"/>
-      <c r="BI10" s="22"/>
-      <c r="BJ10" s="22"/>
-      <c r="BK10" s="22"/>
-      <c r="BL10" s="22"/>
+      <c r="BH10" s="14"/>
+      <c r="BI10" s="14"/>
+      <c r="BJ10" s="14"/>
+      <c r="BK10" s="14"/>
+      <c r="BL10" s="14"/>
     </row>
     <row r="11" spans="1:153" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -4325,7 +4465,7 @@
       <c r="D11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="31" t="s">
         <v>31</v>
       </c>
       <c r="F11" s="12" t="s">
@@ -4334,85 +4474,85 @@
       <c r="G11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="I11" s="14" t="s">
         <v>105</v>
       </c>
       <c r="J11" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="K11" s="23" t="s">
+      <c r="K11" s="14" t="s">
         <v>106</v>
       </c>
       <c r="L11" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="M11" s="23" t="s">
+      <c r="M11" s="14" t="s">
         <v>107</v>
       </c>
       <c r="N11" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="O11" s="23" t="s">
+      <c r="O11" s="14" t="s">
         <v>108</v>
       </c>
       <c r="P11" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="Q11" s="23" t="s">
+      <c r="Q11" s="14" t="s">
         <v>109</v>
       </c>
       <c r="R11" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="S11" s="23"/>
+      <c r="S11" s="14"/>
       <c r="T11" s="14"/>
-      <c r="U11" s="23"/>
+      <c r="U11" s="14"/>
       <c r="V11" s="14"/>
-      <c r="W11" s="23"/>
+      <c r="W11" s="14"/>
       <c r="X11" s="14"/>
-      <c r="Y11" s="23"/>
+      <c r="Y11" s="14"/>
       <c r="Z11" s="14"/>
-      <c r="AA11" s="23"/>
+      <c r="AA11" s="14"/>
       <c r="AB11" s="14"/>
-      <c r="AC11" s="23"/>
+      <c r="AC11" s="14"/>
       <c r="AD11" s="14"/>
-      <c r="AE11" s="23"/>
+      <c r="AE11" s="14"/>
       <c r="AF11" s="14"/>
-      <c r="AG11" s="23"/>
+      <c r="AG11" s="14"/>
       <c r="AH11" s="14"/>
-      <c r="AI11" s="23"/>
+      <c r="AI11" s="14"/>
       <c r="AJ11" s="14"/>
-      <c r="AK11" s="23"/>
+      <c r="AK11" s="14"/>
       <c r="AL11" s="14"/>
-      <c r="AM11" s="23"/>
-      <c r="AN11" s="23"/>
-      <c r="AO11" s="23"/>
-      <c r="AP11" s="23"/>
-      <c r="AQ11" s="23"/>
-      <c r="AR11" s="23"/>
-      <c r="AS11" s="23"/>
-      <c r="AT11" s="23"/>
-      <c r="AU11" s="23"/>
-      <c r="AV11" s="23"/>
-      <c r="AW11" s="23"/>
-      <c r="AX11" s="23"/>
-      <c r="AY11" s="23"/>
-      <c r="AZ11" s="23"/>
-      <c r="BA11" s="23"/>
-      <c r="BB11" s="23"/>
+      <c r="AM11" s="14"/>
+      <c r="AN11" s="14"/>
+      <c r="AO11" s="14"/>
+      <c r="AP11" s="14"/>
+      <c r="AQ11" s="14"/>
+      <c r="AR11" s="14"/>
+      <c r="AS11" s="14"/>
+      <c r="AT11" s="14"/>
+      <c r="AU11" s="14"/>
+      <c r="AV11" s="14"/>
+      <c r="AW11" s="14"/>
+      <c r="AX11" s="14"/>
+      <c r="AY11" s="14"/>
+      <c r="AZ11" s="14"/>
+      <c r="BA11" s="14"/>
+      <c r="BB11" s="14"/>
       <c r="BC11" s="14"/>
-      <c r="BD11" s="22"/>
+      <c r="BD11" s="14"/>
       <c r="BE11" s="14"/>
-      <c r="BF11" s="22"/>
+      <c r="BF11" s="14"/>
       <c r="BG11" s="14"/>
-      <c r="BH11" s="22"/>
-      <c r="BI11" s="22"/>
-      <c r="BJ11" s="22"/>
-      <c r="BK11" s="22"/>
-      <c r="BL11" s="22"/>
+      <c r="BH11" s="14"/>
+      <c r="BI11" s="14"/>
+      <c r="BJ11" s="14"/>
+      <c r="BK11" s="14"/>
+      <c r="BL11" s="14"/>
     </row>
     <row r="12" spans="1:153" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -4425,7 +4565,7 @@
       <c r="D12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="31" t="s">
         <v>31</v>
       </c>
       <c r="F12" s="12" t="s">
@@ -4434,65 +4574,65 @@
       <c r="G12" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="14" t="s">
         <v>93</v>
       </c>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
-      <c r="K12" s="23"/>
+      <c r="K12" s="14"/>
       <c r="L12" s="14"/>
-      <c r="M12" s="23"/>
+      <c r="M12" s="14"/>
       <c r="N12" s="14"/>
-      <c r="O12" s="23"/>
+      <c r="O12" s="14"/>
       <c r="P12" s="14"/>
-      <c r="Q12" s="23"/>
+      <c r="Q12" s="14"/>
       <c r="R12" s="14"/>
-      <c r="S12" s="23"/>
+      <c r="S12" s="14"/>
       <c r="T12" s="14"/>
-      <c r="U12" s="23"/>
+      <c r="U12" s="14"/>
       <c r="V12" s="14"/>
-      <c r="W12" s="23"/>
+      <c r="W12" s="14"/>
       <c r="X12" s="14"/>
-      <c r="Y12" s="23"/>
+      <c r="Y12" s="14"/>
       <c r="Z12" s="14"/>
-      <c r="AA12" s="23"/>
+      <c r="AA12" s="14"/>
       <c r="AB12" s="14"/>
-      <c r="AC12" s="23"/>
+      <c r="AC12" s="14"/>
       <c r="AD12" s="14"/>
-      <c r="AE12" s="23"/>
+      <c r="AE12" s="14"/>
       <c r="AF12" s="14"/>
-      <c r="AG12" s="23"/>
+      <c r="AG12" s="14"/>
       <c r="AH12" s="14"/>
-      <c r="AI12" s="23"/>
+      <c r="AI12" s="14"/>
       <c r="AJ12" s="14"/>
-      <c r="AK12" s="23"/>
+      <c r="AK12" s="14"/>
       <c r="AL12" s="14"/>
-      <c r="AM12" s="23"/>
-      <c r="AN12" s="23"/>
-      <c r="AO12" s="23"/>
-      <c r="AP12" s="23"/>
-      <c r="AQ12" s="23"/>
-      <c r="AR12" s="23"/>
-      <c r="AS12" s="23"/>
-      <c r="AT12" s="23"/>
-      <c r="AU12" s="23"/>
-      <c r="AV12" s="23"/>
-      <c r="AW12" s="23"/>
-      <c r="AX12" s="23"/>
-      <c r="AY12" s="23"/>
-      <c r="AZ12" s="23"/>
-      <c r="BA12" s="23"/>
-      <c r="BB12" s="23"/>
+      <c r="AM12" s="14"/>
+      <c r="AN12" s="14"/>
+      <c r="AO12" s="14"/>
+      <c r="AP12" s="14"/>
+      <c r="AQ12" s="14"/>
+      <c r="AR12" s="14"/>
+      <c r="AS12" s="14"/>
+      <c r="AT12" s="14"/>
+      <c r="AU12" s="14"/>
+      <c r="AV12" s="14"/>
+      <c r="AW12" s="14"/>
+      <c r="AX12" s="14"/>
+      <c r="AY12" s="14"/>
+      <c r="AZ12" s="14"/>
+      <c r="BA12" s="14"/>
+      <c r="BB12" s="14"/>
       <c r="BC12" s="14"/>
-      <c r="BD12" s="22"/>
+      <c r="BD12" s="14"/>
       <c r="BE12" s="14"/>
-      <c r="BF12" s="22"/>
+      <c r="BF12" s="14"/>
       <c r="BG12" s="14"/>
-      <c r="BH12" s="22"/>
-      <c r="BI12" s="22"/>
-      <c r="BJ12" s="22"/>
-      <c r="BK12" s="22"/>
-      <c r="BL12" s="22"/>
+      <c r="BH12" s="14"/>
+      <c r="BI12" s="14"/>
+      <c r="BJ12" s="14"/>
+      <c r="BK12" s="14"/>
+      <c r="BL12" s="14"/>
     </row>
     <row r="13" spans="1:153" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -4505,7 +4645,7 @@
       <c r="D13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="31" t="s">
         <v>31</v>
       </c>
       <c r="F13" s="12" t="s">
@@ -4514,101 +4654,101 @@
       <c r="G13" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="H13" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="14" t="s">
         <v>111</v>
       </c>
       <c r="J13" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="K13" s="23" t="s">
+      <c r="K13" s="14" t="s">
         <v>112</v>
       </c>
       <c r="L13" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="M13" s="23" t="s">
+      <c r="M13" s="14" t="s">
         <v>113</v>
       </c>
       <c r="N13" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="O13" s="23" t="s">
+      <c r="O13" s="14" t="s">
         <v>114</v>
       </c>
       <c r="P13" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="Q13" s="23" t="s">
+      <c r="Q13" s="14" t="s">
         <v>65</v>
       </c>
       <c r="R13" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="S13" s="23" t="s">
+      <c r="S13" s="14" t="s">
         <v>68</v>
       </c>
       <c r="T13" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="U13" s="23" t="s">
+      <c r="U13" s="14" t="s">
         <v>115</v>
       </c>
       <c r="V13" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="W13" s="23" t="s">
+      <c r="W13" s="14" t="s">
         <v>116</v>
       </c>
       <c r="X13" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="Y13" s="23" t="s">
+      <c r="Y13" s="14" t="s">
         <v>117</v>
       </c>
       <c r="Z13" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AA13" s="23"/>
+      <c r="AA13" s="14"/>
       <c r="AB13" s="14"/>
-      <c r="AC13" s="23"/>
+      <c r="AC13" s="14"/>
       <c r="AD13" s="14"/>
-      <c r="AE13" s="23"/>
+      <c r="AE13" s="14"/>
       <c r="AF13" s="14"/>
-      <c r="AG13" s="23"/>
+      <c r="AG13" s="14"/>
       <c r="AH13" s="14"/>
-      <c r="AI13" s="23"/>
+      <c r="AI13" s="14"/>
       <c r="AJ13" s="14"/>
-      <c r="AK13" s="23"/>
+      <c r="AK13" s="14"/>
       <c r="AL13" s="14"/>
-      <c r="AM13" s="23"/>
-      <c r="AN13" s="23"/>
-      <c r="AO13" s="23"/>
-      <c r="AP13" s="23"/>
-      <c r="AQ13" s="23"/>
-      <c r="AR13" s="23"/>
-      <c r="AS13" s="23"/>
-      <c r="AT13" s="23"/>
-      <c r="AU13" s="23"/>
-      <c r="AV13" s="23"/>
-      <c r="AW13" s="23"/>
-      <c r="AX13" s="23"/>
-      <c r="AY13" s="23"/>
-      <c r="AZ13" s="23"/>
-      <c r="BA13" s="23"/>
-      <c r="BB13" s="23"/>
+      <c r="AM13" s="14"/>
+      <c r="AN13" s="14"/>
+      <c r="AO13" s="14"/>
+      <c r="AP13" s="14"/>
+      <c r="AQ13" s="14"/>
+      <c r="AR13" s="14"/>
+      <c r="AS13" s="14"/>
+      <c r="AT13" s="14"/>
+      <c r="AU13" s="14"/>
+      <c r="AV13" s="14"/>
+      <c r="AW13" s="14"/>
+      <c r="AX13" s="14"/>
+      <c r="AY13" s="14"/>
+      <c r="AZ13" s="14"/>
+      <c r="BA13" s="14"/>
+      <c r="BB13" s="14"/>
       <c r="BC13" s="14"/>
-      <c r="BD13" s="22"/>
+      <c r="BD13" s="14"/>
       <c r="BE13" s="14"/>
-      <c r="BF13" s="22"/>
+      <c r="BF13" s="14"/>
       <c r="BG13" s="14"/>
-      <c r="BH13" s="22"/>
-      <c r="BI13" s="22"/>
-      <c r="BJ13" s="22"/>
-      <c r="BK13" s="22"/>
-      <c r="BL13" s="22"/>
+      <c r="BH13" s="14"/>
+      <c r="BI13" s="14"/>
+      <c r="BJ13" s="14"/>
+      <c r="BK13" s="14"/>
+      <c r="BL13" s="14"/>
     </row>
     <row r="14" spans="1:153" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -4621,7 +4761,7 @@
       <c r="D14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="31" t="s">
         <v>31</v>
       </c>
       <c r="F14" s="12" t="s">
@@ -4630,142 +4770,142 @@
       <c r="G14" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="23" t="s">
+      <c r="H14" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="I14" s="23" t="s">
+      <c r="I14" s="14" t="s">
         <v>118</v>
       </c>
       <c r="J14" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="K14" s="23" t="s">
+      <c r="K14" s="14" t="s">
         <v>119</v>
       </c>
       <c r="L14" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="M14" s="23" t="s">
+      <c r="M14" s="14" t="s">
         <v>120</v>
       </c>
       <c r="N14" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="O14" s="23" t="s">
+      <c r="O14" s="14" t="s">
         <v>121</v>
       </c>
       <c r="P14" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="Q14" s="23" t="s">
+      <c r="Q14" s="14" t="s">
         <v>122</v>
       </c>
       <c r="R14" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="S14" s="23" t="s">
+      <c r="S14" s="14" t="s">
         <v>123</v>
       </c>
       <c r="T14" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="U14" s="23" t="s">
+      <c r="U14" s="14" t="s">
         <v>156</v>
       </c>
       <c r="V14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="W14" s="23" t="s">
+      <c r="W14" s="14" t="s">
         <v>124</v>
       </c>
       <c r="X14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="Y14" s="23" t="s">
+      <c r="Y14" s="14" t="s">
         <v>125</v>
       </c>
       <c r="Z14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AA14" s="23" t="s">
+      <c r="AA14" s="14" t="s">
         <v>126</v>
       </c>
       <c r="AB14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AC14" s="23" t="s">
+      <c r="AC14" s="14" t="s">
         <v>127</v>
       </c>
       <c r="AD14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AE14" s="23" t="s">
+      <c r="AE14" s="14" t="s">
         <v>128</v>
       </c>
       <c r="AF14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AG14" s="23" t="s">
+      <c r="AG14" s="14" t="s">
         <v>129</v>
       </c>
       <c r="AH14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AI14" s="23" t="s">
+      <c r="AI14" s="14" t="s">
         <v>130</v>
       </c>
       <c r="AJ14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AK14" s="23" t="s">
+      <c r="AK14" s="14" t="s">
         <v>131</v>
       </c>
       <c r="AL14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AM14" s="23" t="s">
+      <c r="AM14" s="14" t="s">
         <v>132</v>
       </c>
       <c r="AN14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AO14" s="23" t="s">
+      <c r="AO14" s="14" t="s">
         <v>135</v>
       </c>
       <c r="AP14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AQ14" s="23" t="s">
+      <c r="AQ14" s="14" t="s">
         <v>136</v>
       </c>
       <c r="AR14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AS14" s="23" t="s">
+      <c r="AS14" s="14" t="s">
         <v>137</v>
       </c>
       <c r="AT14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AU14" s="23" t="s">
+      <c r="AU14" s="14" t="s">
         <v>112</v>
       </c>
       <c r="AV14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AW14" s="23" t="s">
+      <c r="AW14" s="14" t="s">
         <v>138</v>
       </c>
       <c r="AX14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AY14" s="23" t="s">
+      <c r="AY14" s="14" t="s">
         <v>139</v>
       </c>
       <c r="AZ14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="BA14" s="23" t="s">
+      <c r="BA14" s="14" t="s">
         <v>140</v>
       </c>
       <c r="BB14" s="14" t="s">
@@ -4789,18 +4929,731 @@
       <c r="BH14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="BI14" s="22" t="s">
+      <c r="BI14" s="14" t="s">
         <v>145</v>
       </c>
       <c r="BJ14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="BK14" s="22"/>
-      <c r="BL14" s="22"/>
+      <c r="BK14" s="14"/>
+      <c r="BL14" s="14"/>
+    </row>
+    <row r="15" spans="1:153" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
+      <c r="Y15" s="14"/>
+      <c r="Z15" s="14"/>
+      <c r="AA15" s="14"/>
+      <c r="AB15" s="14"/>
+      <c r="AC15" s="14"/>
+      <c r="AD15" s="14"/>
+      <c r="AE15" s="14"/>
+      <c r="AF15" s="14"/>
+      <c r="AG15" s="14"/>
+      <c r="AH15" s="14"/>
+      <c r="AI15" s="14"/>
+      <c r="AJ15" s="14"/>
+      <c r="AK15" s="14"/>
+      <c r="AL15" s="14"/>
+      <c r="AM15" s="14"/>
+      <c r="AN15" s="14"/>
+      <c r="AO15" s="14"/>
+      <c r="AP15" s="14"/>
+      <c r="AQ15" s="14"/>
+      <c r="AR15" s="14"/>
+      <c r="AS15" s="14"/>
+      <c r="AT15" s="14"/>
+      <c r="AU15" s="14"/>
+      <c r="AV15" s="14"/>
+      <c r="AW15" s="14"/>
+      <c r="AX15" s="14"/>
+      <c r="AY15" s="14"/>
+      <c r="AZ15" s="14"/>
+      <c r="BA15" s="14"/>
+      <c r="BB15" s="14"/>
+      <c r="BC15" s="14"/>
+      <c r="BD15" s="14"/>
+      <c r="BE15" s="14"/>
+      <c r="BF15" s="14"/>
+      <c r="BG15" s="14"/>
+      <c r="BH15" s="14"/>
+      <c r="BI15" s="14"/>
+      <c r="BJ15" s="14"/>
+      <c r="BK15" s="14"/>
+      <c r="BL15" s="14"/>
+      <c r="BM15" s="14"/>
+      <c r="BN15" s="14"/>
+      <c r="BO15" s="14"/>
+      <c r="BP15" s="14"/>
+      <c r="BQ15" s="14"/>
+      <c r="BR15" s="14"/>
+      <c r="BS15" s="14"/>
+      <c r="BT15" s="14"/>
+      <c r="BU15" s="14"/>
+      <c r="BV15" s="14"/>
+      <c r="BW15" s="14"/>
+      <c r="BX15" s="14"/>
+      <c r="BY15" s="14"/>
+      <c r="BZ15" s="14"/>
+      <c r="CA15" s="14"/>
+      <c r="CB15" s="14"/>
+      <c r="CC15" s="14"/>
+      <c r="CD15" s="14"/>
+      <c r="CE15" s="14"/>
+      <c r="CF15" s="14"/>
+      <c r="CG15" s="14"/>
+      <c r="CH15" s="14"/>
+      <c r="CI15" s="14"/>
+      <c r="CJ15" s="14"/>
+      <c r="CK15" s="14"/>
+      <c r="CL15" s="14"/>
+      <c r="CM15" s="14"/>
+      <c r="CN15" s="14"/>
+    </row>
+    <row r="16" spans="1:153" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="M16" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="N16" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="O16" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="P16" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q16" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="R16" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="S16" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="T16" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="U16" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="V16" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="W16" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="X16" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y16" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z16" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA16" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB16" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC16" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="AD16" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE16" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="AF16" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG16" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="AH16" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI16" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="AJ16" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK16" s="14"/>
+      <c r="AL16" s="14"/>
+      <c r="AM16" s="14"/>
+      <c r="AN16" s="14"/>
+      <c r="AO16" s="14"/>
+      <c r="AP16" s="14"/>
+      <c r="AQ16" s="14"/>
+      <c r="AR16" s="14"/>
+      <c r="AS16" s="14"/>
+      <c r="AT16" s="14"/>
+      <c r="AU16" s="14"/>
+      <c r="AV16" s="14"/>
+      <c r="AW16" s="14"/>
+      <c r="AX16" s="14"/>
+      <c r="AY16" s="14"/>
+      <c r="AZ16" s="14"/>
+      <c r="BA16" s="14"/>
+      <c r="BB16" s="14"/>
+      <c r="BD16" s="21"/>
+      <c r="BF16" s="21"/>
+      <c r="BH16" s="21"/>
+      <c r="BI16" s="21"/>
+      <c r="BJ16" s="21"/>
+      <c r="BK16" s="21"/>
+      <c r="BL16" s="21"/>
+    </row>
+    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="N17" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="O17" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="P17" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q17" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="R17" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="S17" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="T17" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="U17" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="V17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="W17" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="X17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y17" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA17" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC17" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="AD17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE17" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="AF17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG17" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="AH17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI17" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="AJ17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK17" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="AL17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM17" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="AN17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO17" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="AP17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ17" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="AR17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AS17" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="AT17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU17" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="AV17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW17" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="AX17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AY17" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="AZ17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA17" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="BB17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="BD17" s="21"/>
+      <c r="BF17" s="21"/>
+      <c r="BH17" s="21"/>
+      <c r="BI17" s="21"/>
+      <c r="BJ17" s="21"/>
+      <c r="BK17" s="21"/>
+      <c r="BL17" s="21"/>
+    </row>
+    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="14"/>
+      <c r="X18" s="14"/>
+      <c r="Y18" s="14"/>
+      <c r="Z18" s="14"/>
+      <c r="AA18" s="14"/>
+      <c r="AB18" s="14"/>
+      <c r="AC18" s="14"/>
+      <c r="AD18" s="14"/>
+      <c r="AE18" s="14"/>
+      <c r="AF18" s="14"/>
+      <c r="AG18" s="14"/>
+      <c r="AH18" s="14"/>
+      <c r="AI18" s="14"/>
+      <c r="AJ18" s="14"/>
+      <c r="AK18" s="14"/>
+      <c r="AL18" s="14"/>
+      <c r="AM18" s="14"/>
+      <c r="AN18" s="14"/>
+      <c r="AO18" s="14"/>
+      <c r="AP18" s="14"/>
+      <c r="AQ18" s="14"/>
+      <c r="AR18" s="14"/>
+      <c r="AS18" s="14"/>
+      <c r="AT18" s="14"/>
+      <c r="AU18" s="14"/>
+      <c r="AV18" s="14"/>
+      <c r="AW18" s="14"/>
+      <c r="AX18" s="14"/>
+      <c r="AY18" s="14"/>
+      <c r="AZ18" s="14"/>
+      <c r="BA18" s="14"/>
+      <c r="BB18" s="14"/>
+      <c r="BD18" s="21"/>
+      <c r="BF18" s="21"/>
+      <c r="BH18" s="21"/>
+      <c r="BI18" s="21"/>
+      <c r="BJ18" s="21"/>
+      <c r="BK18" s="21"/>
+      <c r="BL18" s="21"/>
+    </row>
+    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="L19" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="M19" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="N19" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
+      <c r="U19" s="14"/>
+      <c r="V19" s="14"/>
+      <c r="W19" s="14"/>
+      <c r="X19" s="14"/>
+      <c r="Y19" s="14"/>
+      <c r="Z19" s="14"/>
+      <c r="AA19" s="14"/>
+      <c r="AB19" s="14"/>
+      <c r="AC19" s="14"/>
+      <c r="AD19" s="14"/>
+      <c r="AE19" s="14"/>
+      <c r="AF19" s="14"/>
+      <c r="AG19" s="14"/>
+      <c r="AH19" s="14"/>
+      <c r="AI19" s="14"/>
+      <c r="AJ19" s="14"/>
+      <c r="AK19" s="14"/>
+      <c r="AL19" s="14"/>
+      <c r="AM19" s="14"/>
+      <c r="AN19" s="14"/>
+      <c r="AO19" s="14"/>
+      <c r="AP19" s="14"/>
+      <c r="AQ19" s="14"/>
+      <c r="AR19" s="14"/>
+      <c r="AS19" s="14"/>
+      <c r="AT19" s="14"/>
+      <c r="AU19" s="14"/>
+      <c r="AV19" s="14"/>
+      <c r="AW19" s="14"/>
+      <c r="AX19" s="14"/>
+      <c r="AY19" s="14"/>
+      <c r="AZ19" s="14"/>
+      <c r="BA19" s="14"/>
+      <c r="BB19" s="14"/>
+      <c r="BD19" s="21"/>
+      <c r="BF19" s="21"/>
+      <c r="BH19" s="21"/>
+      <c r="BI19" s="21"/>
+      <c r="BJ19" s="21"/>
+      <c r="BK19" s="21"/>
+      <c r="BL19" s="21"/>
+    </row>
+    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="M20" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="N20" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="O20" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="P20" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q20" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="R20" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="S20" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="T20" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="U20" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="V20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="W20" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="X20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y20" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="Z20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA20" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC20" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE20" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG20" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI20" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK20" s="14"/>
+      <c r="AL20" s="14"/>
+      <c r="AM20" s="14"/>
+      <c r="AN20" s="14"/>
+      <c r="AO20" s="14"/>
+      <c r="AP20" s="14"/>
+      <c r="AQ20" s="14"/>
+      <c r="AR20" s="14"/>
+      <c r="AS20" s="14"/>
+      <c r="AT20" s="14"/>
+      <c r="AU20" s="14"/>
+      <c r="AV20" s="14"/>
+      <c r="AW20" s="14"/>
+      <c r="AX20" s="14"/>
+      <c r="AY20" s="14"/>
+      <c r="AZ20" s="14"/>
+      <c r="BA20" s="14"/>
+      <c r="BB20" s="14"/>
+      <c r="BD20" s="21"/>
+      <c r="BF20" s="21"/>
+      <c r="BH20" s="21"/>
+      <c r="BI20" s="21"/>
+      <c r="BJ20" s="21"/>
+      <c r="BK20" s="21"/>
+      <c r="BL20" s="21"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T3:T14 AD3:AD14 V3:V14 AB3:AB14 Z3:Z14 N3:N14 X3:X14 J3:J14 P3:P14 R3:R14 AF3:AF14 AH3:AH14 AL3:AL14 AJ3:AJ14 I12 I9 AN14 AP14 AR14 AT14 AV14 AX14 AZ14 BB14 L3:L14 BD14 BF14 BH14 BJ14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T3:T15 AD3:AD14 V3:V15 AB3:AB15 Z3:Z15 N3:N15 X3:X15 J3:J15 P3:P15 R3:R15 AF3:AF14 AH3:AH14 AL3:AL14 AJ3:AJ14 I12 I9 AN14 AP14 AR14 AT14 AV14 AX14 AZ14 BB14 L3:L15 BD14 BF14 BH14 BJ14">
       <formula1>"Not Started,In Progress,Implemented"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4817,18 +5670,14 @@
     <hyperlink ref="E12" r:id="rId10"/>
     <hyperlink ref="E13" r:id="rId11"/>
     <hyperlink ref="E14" r:id="rId12"/>
+    <hyperlink ref="E15" r:id="rId13"/>
+    <hyperlink ref="E16:E20" r:id="rId14" display="https://hcm-aufsn4x0cba.oracleoutsourcing.com/hcmCore/faces/FuseWelcome"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Fields!$A$11:$M$11</xm:f>
-          </x14:formula1>
-          <xm:sqref>H3:H14</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="20">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Fields!$A$15:$A$25</xm:f>
@@ -4889,6 +5738,66 @@
           </x14:formula1>
           <xm:sqref>I14 K14 M14 O14 Q14 S14 U14 W14 Y14 AA14 AC14 AE14 AG14 AI14 AK14 AM14 AO14 AQ14 AS14 AU14 AW14 AY14 BA14 BC14 BE14 BG14 BI14</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Fields!$A$11:$M$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>H3:H15</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Fields!$A$11:$R$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>H16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Fields!$A$11:$R$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>H17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Fields!$A$11:$R$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>H18</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Fields!$A$11:$R$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>H19</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Fields!$A$11:$R$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>H20</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Fields!$C$14:$P$14</xm:f>
+          </x14:formula1>
+          <xm:sqref>I16 K16 M16 O16 Q16 S16 U16 W16 Y16 AA16 AC16 AE16 AG16 AI16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Fields!$C$15:$Y$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>I17 K17 M17 O17 Q17 S17 U17 W17 Y17 AA17 AY17 AC17 BA17 AE17 AG17 AI17 AK17 AM17 AO17 AQ17 AS17 AU17 AW17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Fields!$C$17:$E$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>I19 K19 M19</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Fields!$C$18:$P$18</xm:f>
+          </x14:formula1>
+          <xm:sqref>I20 K20 M20 O20 Q20 S20 U20 W20 Y20 AA20 AC20 AE20 AG20 AI20</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -4900,8 +5809,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AE118"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+    <sheetView topLeftCell="M7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4914,123 +5823,123 @@
     <col min="6" max="6" width="19.140625" style="7" customWidth="1"/>
     <col min="7" max="7" width="19.5703125" style="7" customWidth="1"/>
     <col min="8" max="8" width="19.140625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" style="24" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" style="21" customWidth="1"/>
     <col min="10" max="10" width="19.140625" style="7" customWidth="1"/>
     <col min="11" max="11" width="23.5703125" style="7" customWidth="1"/>
     <col min="12" max="12" width="19.140625" style="7" customWidth="1"/>
     <col min="13" max="13" width="29.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" style="7" customWidth="1"/>
+    <col min="14" max="14" width="28.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="23.5703125" style="7" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" style="7" customWidth="1"/>
-    <col min="17" max="17" width="23.5703125" style="24" customWidth="1"/>
-    <col min="18" max="18" width="19.140625" style="7" customWidth="1"/>
+    <col min="16" max="16" width="34.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="23.5703125" style="7" customWidth="1"/>
     <col min="20" max="20" width="19.140625" style="7" customWidth="1"/>
-    <col min="21" max="21" width="23.5703125" style="24" customWidth="1"/>
+    <col min="21" max="21" width="23.5703125" style="21" customWidth="1"/>
     <col min="22" max="22" width="23.5703125" style="7" customWidth="1"/>
     <col min="23" max="23" width="19.140625" style="7" customWidth="1"/>
     <col min="24" max="24" width="20.28515625" style="7" customWidth="1"/>
     <col min="25" max="25" width="19.140625" style="7" customWidth="1"/>
-    <col min="26" max="27" width="23.5703125" style="24" customWidth="1"/>
-    <col min="28" max="28" width="25.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="29.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="29.140625" style="24" customWidth="1"/>
-    <col min="31" max="31" width="29.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="24"/>
+    <col min="26" max="27" width="23.5703125" style="21" customWidth="1"/>
+    <col min="28" max="28" width="25.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="29.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="29.140625" style="21" customWidth="1"/>
+    <col min="31" max="31" width="29.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="28" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:31" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="P1" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="Q1" s="28" t="s">
+      <c r="Q1" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="R1" s="27" t="s">
+      <c r="R1" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="S1" s="26" t="s">
+      <c r="S1" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="T1" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="U1" s="28" t="s">
+      <c r="U1" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="V1" s="26" t="s">
+      <c r="V1" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="W1" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="X1" s="26" t="s">
+      <c r="X1" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="Y1" s="27" t="s">
+      <c r="Y1" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="Z1" s="26" t="s">
+      <c r="Z1" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="AA1" s="28" t="s">
+      <c r="AA1" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="AB1" s="28" t="s">
+      <c r="AB1" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="AC1" s="26" t="s">
+      <c r="AC1" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="AD1" s="26" t="s">
+      <c r="AD1" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="AE1" s="28" t="s">
+      <c r="AE1" s="25" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5059,7 +5968,7 @@
       <c r="H2" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="21" t="s">
         <v>65</v>
       </c>
       <c r="J2" s="7" t="s">
@@ -5083,7 +5992,7 @@
       <c r="P2" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="24" t="s">
+      <c r="Q2" s="21" t="s">
         <v>133</v>
       </c>
       <c r="R2" s="7" t="s">
@@ -5107,14 +6016,14 @@
       <c r="Y2" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="AB2" s="24" t="s">
+      <c r="AB2" s="21" t="s">
         <v>111</v>
       </c>
       <c r="AC2" s="7" t="s">
         <v>150</v>
       </c>
       <c r="AD2" s="7"/>
-      <c r="AE2" s="24" t="s">
+      <c r="AE2" s="21" t="s">
         <v>151</v>
       </c>
     </row>
@@ -5143,7 +6052,7 @@
       <c r="H3" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="21" t="s">
         <v>66</v>
       </c>
       <c r="J3" s="7" t="s">
@@ -5161,7 +6070,7 @@
       <c r="N3" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="Q3" s="24" t="s">
+      <c r="Q3" s="21" t="s">
         <v>74</v>
       </c>
       <c r="R3" s="7" t="s">
@@ -5185,7 +6094,7 @@
       <c r="Y3" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="AB3" s="24" t="s">
+      <c r="AB3" s="21" t="s">
         <v>112</v>
       </c>
       <c r="AC3" s="7" t="s">
@@ -5242,7 +6151,7 @@
       <c r="Y4" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="AB4" s="24" t="s">
+      <c r="AB4" s="21" t="s">
         <v>113</v>
       </c>
     </row>
@@ -5289,7 +6198,7 @@
       <c r="Y5" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="AB5" s="24" t="s">
+      <c r="AB5" s="21" t="s">
         <v>114</v>
       </c>
     </row>
@@ -5324,7 +6233,7 @@
       <c r="W6" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="AB6" s="24" t="s">
+      <c r="AB6" s="21" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5347,7 +6256,7 @@
       <c r="W7" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="AB7" s="24" t="s">
+      <c r="AB7" s="21" t="s">
         <v>68</v>
       </c>
     </row>
@@ -5385,138 +6294,376 @@
       </c>
     </row>
     <row r="11" spans="1:31" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="H11" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="I11" s="26" t="s">
+      <c r="I11" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="J11" s="28" t="s">
+      <c r="J11" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="K11" s="28" t="s">
+      <c r="K11" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="L11" s="26" t="s">
+      <c r="L11" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="M11" s="28" t="s">
+      <c r="M11" s="25" t="s">
         <v>147</v>
       </c>
+      <c r="N11" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="P11" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q11" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="R11" s="14" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="23" t="s">
         <v>14</v>
       </c>
+      <c r="C14" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="M14" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="N14" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="O14" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="P14" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>53</v>
       </c>
+      <c r="C15" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="L15" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="O15" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="P15" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q15" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="R15" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="S15" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="T15" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="U15" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="V15" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="W15" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="X15" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="Y15" s="14" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="14"/>
+      <c r="X16" s="14"/>
+      <c r="Y16" s="14"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C17" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="14"/>
+      <c r="V17" s="14"/>
+      <c r="W17" s="14"/>
+      <c r="X17" s="14"/>
+      <c r="Y17" s="14"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C18" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="M18" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="N18" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="O18" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="P18" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="14"/>
+      <c r="X18" s="14"/>
+      <c r="Y18" s="14"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A26" s="23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A32" s="23" t="s">
         <v>64</v>
       </c>
     </row>
@@ -5531,7 +6678,7 @@
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="26" t="s">
+      <c r="A35" s="23" t="s">
         <v>67</v>
       </c>
     </row>
@@ -5611,7 +6758,7 @@
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="26" t="s">
+      <c r="A51" s="23" t="s">
         <v>82</v>
       </c>
     </row>
@@ -5626,7 +6773,7 @@
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="26" t="s">
+      <c r="A54" s="23" t="s">
         <v>83</v>
       </c>
     </row>
@@ -5656,12 +6803,12 @@
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="26" t="s">
+      <c r="A60" s="23" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="26" t="s">
+      <c r="A61" s="23" t="s">
         <v>91</v>
       </c>
     </row>
@@ -5716,62 +6863,62 @@
       </c>
     </row>
     <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="26" t="s">
+      <c r="A72" s="23" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A73" s="30" t="s">
+      <c r="A73" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="B73" s="24"/>
-      <c r="C73" s="24"/>
-      <c r="D73" s="24"/>
-      <c r="E73" s="24"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="21"/>
+      <c r="D73" s="21"/>
+      <c r="E73" s="21"/>
     </row>
     <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="30" t="s">
+      <c r="A74" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="B74" s="24"/>
-      <c r="C74" s="24"/>
-      <c r="D74" s="24"/>
-      <c r="E74" s="29"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="21"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="26"/>
     </row>
     <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="30" t="s">
+      <c r="A75" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="B75" s="24"/>
-      <c r="C75" s="24"/>
-      <c r="D75" s="29"/>
-      <c r="E75" s="29"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="26"/>
+      <c r="E75" s="26"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="30" t="s">
+      <c r="A76" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="B76" s="24"/>
-      <c r="C76" s="29"/>
-      <c r="D76" s="29"/>
-      <c r="E76" s="29"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="26"/>
+      <c r="D76" s="26"/>
+      <c r="E76" s="26"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="30" t="s">
+      <c r="A77" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="B77" s="29"/>
-      <c r="C77" s="29"/>
-      <c r="D77" s="29"/>
-      <c r="E77" s="29"/>
+      <c r="B77" s="26"/>
+      <c r="C77" s="26"/>
+      <c r="D77" s="26"/>
+      <c r="E77" s="26"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="26" t="s">
+      <c r="A78" s="23" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="26" t="s">
+      <c r="A80" s="23" t="s">
         <v>94</v>
       </c>
     </row>
@@ -5809,7 +6956,7 @@
       <c r="A87" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B87" s="24"/>
+      <c r="B87" s="21"/>
     </row>
     <row r="88" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
@@ -5822,805 +6969,805 @@
       </c>
     </row>
     <row r="90" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A90" s="26" t="s">
+      <c r="A90" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="B90" s="24"/>
+      <c r="B90" s="21"/>
     </row>
     <row r="91" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A91" s="25" t="s">
+      <c r="A91" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="B91" s="24"/>
-      <c r="C91" s="24"/>
-      <c r="D91" s="24"/>
-      <c r="E91" s="24"/>
-      <c r="F91" s="24"/>
-      <c r="G91" s="24"/>
-      <c r="H91" s="24"/>
-      <c r="J91" s="24"/>
-      <c r="K91" s="24"/>
-      <c r="L91" s="24"/>
-      <c r="M91" s="24"/>
-      <c r="N91" s="24"/>
-      <c r="O91" s="24"/>
-      <c r="P91" s="24"/>
-      <c r="R91" s="24"/>
-      <c r="S91" s="24"/>
-      <c r="T91" s="24"/>
-      <c r="V91" s="24"/>
-      <c r="W91" s="24"/>
-      <c r="X91" s="24"/>
-      <c r="Y91" s="24"/>
+      <c r="B91" s="21"/>
+      <c r="C91" s="21"/>
+      <c r="D91" s="21"/>
+      <c r="E91" s="21"/>
+      <c r="F91" s="21"/>
+      <c r="G91" s="21"/>
+      <c r="H91" s="21"/>
+      <c r="J91" s="21"/>
+      <c r="K91" s="21"/>
+      <c r="L91" s="21"/>
+      <c r="M91" s="21"/>
+      <c r="N91" s="21"/>
+      <c r="O91" s="21"/>
+      <c r="P91" s="21"/>
+      <c r="R91" s="21"/>
+      <c r="S91" s="21"/>
+      <c r="T91" s="21"/>
+      <c r="V91" s="21"/>
+      <c r="W91" s="21"/>
+      <c r="X91" s="21"/>
+      <c r="Y91" s="21"/>
     </row>
     <row r="92" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A92" s="25" t="s">
+      <c r="A92" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="B92" s="24"/>
-      <c r="C92" s="24"/>
-      <c r="D92" s="24"/>
-      <c r="E92" s="24"/>
-      <c r="F92" s="24"/>
-      <c r="G92" s="24"/>
-      <c r="H92" s="24"/>
-      <c r="J92" s="24"/>
-      <c r="K92" s="24"/>
-      <c r="L92" s="24"/>
-      <c r="M92" s="24"/>
-      <c r="N92" s="24"/>
-      <c r="O92" s="24"/>
-      <c r="P92" s="24"/>
-      <c r="R92" s="24"/>
-      <c r="S92" s="24"/>
-      <c r="T92" s="24"/>
-      <c r="V92" s="24"/>
-      <c r="W92" s="24"/>
-      <c r="X92" s="24"/>
-      <c r="Y92" s="24"/>
+      <c r="B92" s="21"/>
+      <c r="C92" s="21"/>
+      <c r="D92" s="21"/>
+      <c r="E92" s="21"/>
+      <c r="F92" s="21"/>
+      <c r="G92" s="21"/>
+      <c r="H92" s="21"/>
+      <c r="J92" s="21"/>
+      <c r="K92" s="21"/>
+      <c r="L92" s="21"/>
+      <c r="M92" s="21"/>
+      <c r="N92" s="21"/>
+      <c r="O92" s="21"/>
+      <c r="P92" s="21"/>
+      <c r="R92" s="21"/>
+      <c r="S92" s="21"/>
+      <c r="T92" s="21"/>
+      <c r="V92" s="21"/>
+      <c r="W92" s="21"/>
+      <c r="X92" s="21"/>
+      <c r="Y92" s="21"/>
     </row>
     <row r="93" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A93" s="25" t="s">
+      <c r="A93" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="B93" s="24"/>
-      <c r="C93" s="24"/>
-      <c r="D93" s="24"/>
-      <c r="E93" s="24"/>
-      <c r="F93" s="24"/>
-      <c r="G93" s="24"/>
-      <c r="H93" s="24"/>
-      <c r="J93" s="24"/>
-      <c r="K93" s="24"/>
-      <c r="L93" s="24"/>
-      <c r="M93" s="24"/>
-      <c r="N93" s="24"/>
-      <c r="O93" s="24"/>
-      <c r="P93" s="24"/>
-      <c r="R93" s="24"/>
-      <c r="S93" s="24"/>
-      <c r="T93" s="24"/>
-      <c r="V93" s="24"/>
-      <c r="W93" s="24"/>
-      <c r="X93" s="24"/>
-      <c r="Y93" s="24"/>
-      <c r="AA93" s="32"/>
+      <c r="B93" s="21"/>
+      <c r="C93" s="21"/>
+      <c r="D93" s="21"/>
+      <c r="E93" s="21"/>
+      <c r="F93" s="21"/>
+      <c r="G93" s="21"/>
+      <c r="H93" s="21"/>
+      <c r="J93" s="21"/>
+      <c r="K93" s="21"/>
+      <c r="L93" s="21"/>
+      <c r="M93" s="21"/>
+      <c r="N93" s="21"/>
+      <c r="O93" s="21"/>
+      <c r="P93" s="21"/>
+      <c r="R93" s="21"/>
+      <c r="S93" s="21"/>
+      <c r="T93" s="21"/>
+      <c r="V93" s="21"/>
+      <c r="W93" s="21"/>
+      <c r="X93" s="21"/>
+      <c r="Y93" s="21"/>
+      <c r="AA93" s="29"/>
     </row>
     <row r="94" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A94" s="25" t="s">
+      <c r="A94" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="B94" s="24"/>
-      <c r="C94" s="24"/>
-      <c r="D94" s="24"/>
-      <c r="E94" s="24"/>
-      <c r="F94" s="24"/>
-      <c r="G94" s="24"/>
-      <c r="H94" s="24"/>
-      <c r="J94" s="24"/>
-      <c r="K94" s="24"/>
-      <c r="L94" s="24"/>
-      <c r="M94" s="24"/>
-      <c r="N94" s="24"/>
-      <c r="O94" s="24"/>
-      <c r="P94" s="24"/>
-      <c r="R94" s="24"/>
-      <c r="S94" s="24"/>
-      <c r="T94" s="24"/>
-      <c r="V94" s="24"/>
-      <c r="W94" s="24"/>
-      <c r="X94" s="24"/>
-      <c r="Y94" s="24"/>
-      <c r="Z94" s="31"/>
-      <c r="AA94" s="32"/>
+      <c r="B94" s="21"/>
+      <c r="C94" s="21"/>
+      <c r="D94" s="21"/>
+      <c r="E94" s="21"/>
+      <c r="F94" s="21"/>
+      <c r="G94" s="21"/>
+      <c r="H94" s="21"/>
+      <c r="J94" s="21"/>
+      <c r="K94" s="21"/>
+      <c r="L94" s="21"/>
+      <c r="M94" s="21"/>
+      <c r="N94" s="21"/>
+      <c r="O94" s="21"/>
+      <c r="P94" s="21"/>
+      <c r="R94" s="21"/>
+      <c r="S94" s="21"/>
+      <c r="T94" s="21"/>
+      <c r="V94" s="21"/>
+      <c r="W94" s="21"/>
+      <c r="X94" s="21"/>
+      <c r="Y94" s="21"/>
+      <c r="Z94" s="28"/>
+      <c r="AA94" s="29"/>
     </row>
     <row r="95" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A95" s="25" t="s">
+      <c r="A95" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="B95" s="24"/>
-      <c r="C95" s="24"/>
-      <c r="D95" s="24"/>
-      <c r="E95" s="24"/>
-      <c r="F95" s="24"/>
-      <c r="G95" s="24"/>
-      <c r="H95" s="24"/>
-      <c r="J95" s="24"/>
-      <c r="K95" s="24"/>
-      <c r="L95" s="24"/>
-      <c r="M95" s="24"/>
-      <c r="N95" s="24"/>
-      <c r="O95" s="24"/>
-      <c r="P95" s="24"/>
-      <c r="R95" s="24"/>
-      <c r="S95" s="24"/>
-      <c r="T95" s="24"/>
-      <c r="V95" s="24"/>
-      <c r="W95" s="24"/>
-      <c r="X95" s="24"/>
-      <c r="Y95" s="31"/>
-      <c r="Z95" s="31"/>
-      <c r="AA95" s="32"/>
+      <c r="B95" s="21"/>
+      <c r="C95" s="21"/>
+      <c r="D95" s="21"/>
+      <c r="E95" s="21"/>
+      <c r="F95" s="21"/>
+      <c r="G95" s="21"/>
+      <c r="H95" s="21"/>
+      <c r="J95" s="21"/>
+      <c r="K95" s="21"/>
+      <c r="L95" s="21"/>
+      <c r="M95" s="21"/>
+      <c r="N95" s="21"/>
+      <c r="O95" s="21"/>
+      <c r="P95" s="21"/>
+      <c r="R95" s="21"/>
+      <c r="S95" s="21"/>
+      <c r="T95" s="21"/>
+      <c r="V95" s="21"/>
+      <c r="W95" s="21"/>
+      <c r="X95" s="21"/>
+      <c r="Y95" s="28"/>
+      <c r="Z95" s="28"/>
+      <c r="AA95" s="29"/>
     </row>
     <row r="96" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A96" s="25" t="s">
+      <c r="A96" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="B96" s="24"/>
-      <c r="C96" s="24"/>
-      <c r="D96" s="24"/>
-      <c r="E96" s="24"/>
-      <c r="F96" s="24"/>
-      <c r="G96" s="24"/>
-      <c r="H96" s="24"/>
-      <c r="J96" s="24"/>
-      <c r="K96" s="24"/>
-      <c r="L96" s="24"/>
-      <c r="M96" s="24"/>
-      <c r="N96" s="24"/>
-      <c r="O96" s="24"/>
-      <c r="P96" s="24"/>
-      <c r="R96" s="24"/>
-      <c r="S96" s="24"/>
-      <c r="T96" s="24"/>
-      <c r="V96" s="24"/>
-      <c r="W96" s="24"/>
-      <c r="X96" s="31"/>
-      <c r="Y96" s="31"/>
-      <c r="Z96" s="31"/>
-      <c r="AA96" s="32"/>
+      <c r="B96" s="21"/>
+      <c r="C96" s="21"/>
+      <c r="D96" s="21"/>
+      <c r="E96" s="21"/>
+      <c r="F96" s="21"/>
+      <c r="G96" s="21"/>
+      <c r="H96" s="21"/>
+      <c r="J96" s="21"/>
+      <c r="K96" s="21"/>
+      <c r="L96" s="21"/>
+      <c r="M96" s="21"/>
+      <c r="N96" s="21"/>
+      <c r="O96" s="21"/>
+      <c r="P96" s="21"/>
+      <c r="R96" s="21"/>
+      <c r="S96" s="21"/>
+      <c r="T96" s="21"/>
+      <c r="V96" s="21"/>
+      <c r="W96" s="21"/>
+      <c r="X96" s="28"/>
+      <c r="Y96" s="28"/>
+      <c r="Z96" s="28"/>
+      <c r="AA96" s="29"/>
     </row>
     <row r="97" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A97" s="25" t="s">
+      <c r="A97" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="B97" s="24"/>
-      <c r="C97" s="24"/>
-      <c r="D97" s="24"/>
-      <c r="E97" s="24"/>
-      <c r="F97" s="24"/>
-      <c r="G97" s="24"/>
-      <c r="H97" s="24"/>
-      <c r="J97" s="24"/>
-      <c r="K97" s="24"/>
-      <c r="L97" s="24"/>
-      <c r="M97" s="24"/>
-      <c r="N97" s="24"/>
-      <c r="O97" s="24"/>
-      <c r="P97" s="24"/>
-      <c r="R97" s="24"/>
-      <c r="S97" s="24"/>
-      <c r="T97" s="24"/>
-      <c r="V97" s="24"/>
-      <c r="W97" s="29"/>
-      <c r="X97" s="31"/>
-      <c r="Y97" s="31"/>
-      <c r="Z97" s="31"/>
-      <c r="AA97" s="32"/>
+      <c r="B97" s="21"/>
+      <c r="C97" s="21"/>
+      <c r="D97" s="21"/>
+      <c r="E97" s="21"/>
+      <c r="F97" s="21"/>
+      <c r="G97" s="21"/>
+      <c r="H97" s="21"/>
+      <c r="J97" s="21"/>
+      <c r="K97" s="21"/>
+      <c r="L97" s="21"/>
+      <c r="M97" s="21"/>
+      <c r="N97" s="21"/>
+      <c r="O97" s="21"/>
+      <c r="P97" s="21"/>
+      <c r="R97" s="21"/>
+      <c r="S97" s="21"/>
+      <c r="T97" s="21"/>
+      <c r="V97" s="21"/>
+      <c r="W97" s="26"/>
+      <c r="X97" s="28"/>
+      <c r="Y97" s="28"/>
+      <c r="Z97" s="28"/>
+      <c r="AA97" s="29"/>
     </row>
     <row r="98" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A98" s="25" t="s">
+      <c r="A98" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="B98" s="24"/>
-      <c r="C98" s="24"/>
-      <c r="D98" s="24"/>
-      <c r="E98" s="24"/>
-      <c r="F98" s="24"/>
-      <c r="G98" s="24"/>
-      <c r="H98" s="24"/>
-      <c r="J98" s="24"/>
-      <c r="K98" s="24"/>
-      <c r="L98" s="24"/>
-      <c r="M98" s="24"/>
-      <c r="N98" s="24"/>
-      <c r="O98" s="24"/>
-      <c r="P98" s="24"/>
-      <c r="R98" s="24"/>
-      <c r="S98" s="24"/>
-      <c r="T98" s="24"/>
-      <c r="V98" s="29"/>
-      <c r="W98" s="29"/>
-      <c r="X98" s="31"/>
-      <c r="Y98" s="31"/>
-      <c r="Z98" s="31"/>
-      <c r="AA98" s="32"/>
+      <c r="B98" s="21"/>
+      <c r="C98" s="21"/>
+      <c r="D98" s="21"/>
+      <c r="E98" s="21"/>
+      <c r="F98" s="21"/>
+      <c r="G98" s="21"/>
+      <c r="H98" s="21"/>
+      <c r="J98" s="21"/>
+      <c r="K98" s="21"/>
+      <c r="L98" s="21"/>
+      <c r="M98" s="21"/>
+      <c r="N98" s="21"/>
+      <c r="O98" s="21"/>
+      <c r="P98" s="21"/>
+      <c r="R98" s="21"/>
+      <c r="S98" s="21"/>
+      <c r="T98" s="21"/>
+      <c r="V98" s="26"/>
+      <c r="W98" s="26"/>
+      <c r="X98" s="28"/>
+      <c r="Y98" s="28"/>
+      <c r="Z98" s="28"/>
+      <c r="AA98" s="29"/>
     </row>
     <row r="99" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A99" s="25" t="s">
+      <c r="A99" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="B99" s="24"/>
-      <c r="C99" s="24"/>
-      <c r="D99" s="24"/>
-      <c r="E99" s="24"/>
-      <c r="F99" s="24"/>
-      <c r="G99" s="24"/>
-      <c r="H99" s="24"/>
-      <c r="J99" s="24"/>
-      <c r="K99" s="24"/>
-      <c r="L99" s="24"/>
-      <c r="M99" s="24"/>
-      <c r="N99" s="24"/>
-      <c r="O99" s="24"/>
-      <c r="P99" s="24"/>
-      <c r="R99" s="24"/>
-      <c r="S99" s="24"/>
-      <c r="T99" s="24"/>
-      <c r="U99" s="29"/>
-      <c r="V99" s="29"/>
-      <c r="W99" s="29"/>
-      <c r="X99" s="31"/>
-      <c r="Y99" s="31"/>
-      <c r="Z99" s="31"/>
-      <c r="AA99" s="32"/>
+      <c r="B99" s="21"/>
+      <c r="C99" s="21"/>
+      <c r="D99" s="21"/>
+      <c r="E99" s="21"/>
+      <c r="F99" s="21"/>
+      <c r="G99" s="21"/>
+      <c r="H99" s="21"/>
+      <c r="J99" s="21"/>
+      <c r="K99" s="21"/>
+      <c r="L99" s="21"/>
+      <c r="M99" s="21"/>
+      <c r="N99" s="21"/>
+      <c r="O99" s="21"/>
+      <c r="P99" s="21"/>
+      <c r="R99" s="21"/>
+      <c r="S99" s="21"/>
+      <c r="T99" s="21"/>
+      <c r="U99" s="26"/>
+      <c r="V99" s="26"/>
+      <c r="W99" s="26"/>
+      <c r="X99" s="28"/>
+      <c r="Y99" s="28"/>
+      <c r="Z99" s="28"/>
+      <c r="AA99" s="29"/>
     </row>
     <row r="100" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A100" s="25" t="s">
+      <c r="A100" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="B100" s="24"/>
-      <c r="C100" s="24"/>
-      <c r="D100" s="24"/>
-      <c r="E100" s="24"/>
-      <c r="F100" s="24"/>
-      <c r="G100" s="24"/>
-      <c r="H100" s="24"/>
-      <c r="J100" s="24"/>
-      <c r="K100" s="24"/>
-      <c r="L100" s="24"/>
-      <c r="M100" s="24"/>
-      <c r="N100" s="24"/>
-      <c r="O100" s="24"/>
-      <c r="P100" s="24"/>
-      <c r="R100" s="24"/>
-      <c r="S100" s="24"/>
-      <c r="T100" s="29"/>
-      <c r="U100" s="29"/>
-      <c r="V100" s="29"/>
-      <c r="W100" s="29"/>
-      <c r="X100" s="31"/>
-      <c r="Y100" s="31"/>
-      <c r="Z100" s="31"/>
-      <c r="AA100" s="32"/>
+      <c r="B100" s="21"/>
+      <c r="C100" s="21"/>
+      <c r="D100" s="21"/>
+      <c r="E100" s="21"/>
+      <c r="F100" s="21"/>
+      <c r="G100" s="21"/>
+      <c r="H100" s="21"/>
+      <c r="J100" s="21"/>
+      <c r="K100" s="21"/>
+      <c r="L100" s="21"/>
+      <c r="M100" s="21"/>
+      <c r="N100" s="21"/>
+      <c r="O100" s="21"/>
+      <c r="P100" s="21"/>
+      <c r="R100" s="21"/>
+      <c r="S100" s="21"/>
+      <c r="T100" s="26"/>
+      <c r="U100" s="26"/>
+      <c r="V100" s="26"/>
+      <c r="W100" s="26"/>
+      <c r="X100" s="28"/>
+      <c r="Y100" s="28"/>
+      <c r="Z100" s="28"/>
+      <c r="AA100" s="29"/>
     </row>
     <row r="101" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A101" s="25" t="s">
+      <c r="A101" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="B101" s="24"/>
-      <c r="C101" s="24"/>
-      <c r="D101" s="24"/>
-      <c r="E101" s="24"/>
-      <c r="F101" s="24"/>
-      <c r="G101" s="24"/>
-      <c r="H101" s="24"/>
-      <c r="J101" s="24"/>
-      <c r="K101" s="24"/>
-      <c r="L101" s="24"/>
-      <c r="M101" s="24"/>
-      <c r="N101" s="24"/>
-      <c r="O101" s="24"/>
-      <c r="P101" s="24"/>
-      <c r="R101" s="24"/>
-      <c r="S101" s="29"/>
-      <c r="T101" s="29"/>
-      <c r="U101" s="29"/>
-      <c r="V101" s="29"/>
-      <c r="W101" s="29"/>
-      <c r="X101" s="31"/>
-      <c r="Y101" s="31"/>
-      <c r="Z101" s="31"/>
-      <c r="AA101" s="32"/>
+      <c r="B101" s="21"/>
+      <c r="C101" s="21"/>
+      <c r="D101" s="21"/>
+      <c r="E101" s="21"/>
+      <c r="F101" s="21"/>
+      <c r="G101" s="21"/>
+      <c r="H101" s="21"/>
+      <c r="J101" s="21"/>
+      <c r="K101" s="21"/>
+      <c r="L101" s="21"/>
+      <c r="M101" s="21"/>
+      <c r="N101" s="21"/>
+      <c r="O101" s="21"/>
+      <c r="P101" s="21"/>
+      <c r="R101" s="21"/>
+      <c r="S101" s="26"/>
+      <c r="T101" s="26"/>
+      <c r="U101" s="26"/>
+      <c r="V101" s="26"/>
+      <c r="W101" s="26"/>
+      <c r="X101" s="28"/>
+      <c r="Y101" s="28"/>
+      <c r="Z101" s="28"/>
+      <c r="AA101" s="29"/>
     </row>
     <row r="102" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A102" s="25" t="s">
+      <c r="A102" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="B102" s="24"/>
-      <c r="C102" s="24"/>
-      <c r="D102" s="24"/>
-      <c r="E102" s="24"/>
-      <c r="F102" s="24"/>
-      <c r="G102" s="24"/>
-      <c r="H102" s="24"/>
-      <c r="J102" s="24"/>
-      <c r="K102" s="24"/>
-      <c r="L102" s="24"/>
-      <c r="M102" s="24"/>
-      <c r="N102" s="24"/>
-      <c r="O102" s="24"/>
-      <c r="P102" s="24"/>
-      <c r="R102" s="29"/>
-      <c r="S102" s="29"/>
-      <c r="T102" s="29"/>
-      <c r="U102" s="29"/>
-      <c r="V102" s="29"/>
-      <c r="W102" s="29"/>
-      <c r="X102" s="31"/>
-      <c r="Y102" s="31"/>
-      <c r="Z102" s="31"/>
-      <c r="AA102" s="32"/>
+      <c r="B102" s="21"/>
+      <c r="C102" s="21"/>
+      <c r="D102" s="21"/>
+      <c r="E102" s="21"/>
+      <c r="F102" s="21"/>
+      <c r="G102" s="21"/>
+      <c r="H102" s="21"/>
+      <c r="J102" s="21"/>
+      <c r="K102" s="21"/>
+      <c r="L102" s="21"/>
+      <c r="M102" s="21"/>
+      <c r="N102" s="21"/>
+      <c r="O102" s="21"/>
+      <c r="P102" s="21"/>
+      <c r="R102" s="26"/>
+      <c r="S102" s="26"/>
+      <c r="T102" s="26"/>
+      <c r="U102" s="26"/>
+      <c r="V102" s="26"/>
+      <c r="W102" s="26"/>
+      <c r="X102" s="28"/>
+      <c r="Y102" s="28"/>
+      <c r="Z102" s="28"/>
+      <c r="AA102" s="29"/>
     </row>
     <row r="103" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A103" s="25" t="s">
+      <c r="A103" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="B103" s="24"/>
-      <c r="C103" s="24"/>
-      <c r="D103" s="24"/>
-      <c r="E103" s="24"/>
-      <c r="F103" s="24"/>
-      <c r="G103" s="24"/>
-      <c r="H103" s="24"/>
-      <c r="J103" s="24"/>
-      <c r="K103" s="24"/>
-      <c r="L103" s="24"/>
-      <c r="M103" s="24"/>
-      <c r="N103" s="24"/>
-      <c r="O103" s="24"/>
-      <c r="P103" s="24"/>
-      <c r="Q103" s="29"/>
-      <c r="R103" s="29"/>
-      <c r="S103" s="29"/>
-      <c r="T103" s="29"/>
-      <c r="U103" s="29"/>
-      <c r="V103" s="29"/>
-      <c r="W103" s="29"/>
-      <c r="X103" s="31"/>
-      <c r="Y103" s="31"/>
-      <c r="Z103" s="31"/>
-      <c r="AA103" s="32"/>
+      <c r="B103" s="21"/>
+      <c r="C103" s="21"/>
+      <c r="D103" s="21"/>
+      <c r="E103" s="21"/>
+      <c r="F103" s="21"/>
+      <c r="G103" s="21"/>
+      <c r="H103" s="21"/>
+      <c r="J103" s="21"/>
+      <c r="K103" s="21"/>
+      <c r="L103" s="21"/>
+      <c r="M103" s="21"/>
+      <c r="N103" s="21"/>
+      <c r="O103" s="21"/>
+      <c r="P103" s="21"/>
+      <c r="Q103" s="26"/>
+      <c r="R103" s="26"/>
+      <c r="S103" s="26"/>
+      <c r="T103" s="26"/>
+      <c r="U103" s="26"/>
+      <c r="V103" s="26"/>
+      <c r="W103" s="26"/>
+      <c r="X103" s="28"/>
+      <c r="Y103" s="28"/>
+      <c r="Z103" s="28"/>
+      <c r="AA103" s="29"/>
     </row>
     <row r="104" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A104" s="25" t="s">
+      <c r="A104" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="B104" s="24"/>
-      <c r="C104" s="24"/>
-      <c r="D104" s="24"/>
-      <c r="E104" s="24"/>
-      <c r="F104" s="24"/>
-      <c r="G104" s="24"/>
-      <c r="H104" s="24"/>
-      <c r="J104" s="24"/>
-      <c r="K104" s="24"/>
-      <c r="L104" s="24"/>
-      <c r="M104" s="24"/>
-      <c r="N104" s="24"/>
-      <c r="O104" s="24"/>
-      <c r="P104" s="29"/>
-      <c r="Q104" s="29"/>
-      <c r="R104" s="29"/>
-      <c r="S104" s="29"/>
-      <c r="T104" s="29"/>
-      <c r="U104" s="29"/>
-      <c r="V104" s="29"/>
-      <c r="W104" s="29"/>
-      <c r="X104" s="31"/>
-      <c r="Y104" s="31"/>
-      <c r="Z104" s="31"/>
-      <c r="AA104" s="32"/>
+      <c r="B104" s="21"/>
+      <c r="C104" s="21"/>
+      <c r="D104" s="21"/>
+      <c r="E104" s="21"/>
+      <c r="F104" s="21"/>
+      <c r="G104" s="21"/>
+      <c r="H104" s="21"/>
+      <c r="J104" s="21"/>
+      <c r="K104" s="21"/>
+      <c r="L104" s="21"/>
+      <c r="M104" s="21"/>
+      <c r="N104" s="21"/>
+      <c r="O104" s="21"/>
+      <c r="P104" s="26"/>
+      <c r="Q104" s="26"/>
+      <c r="R104" s="26"/>
+      <c r="S104" s="26"/>
+      <c r="T104" s="26"/>
+      <c r="U104" s="26"/>
+      <c r="V104" s="26"/>
+      <c r="W104" s="26"/>
+      <c r="X104" s="28"/>
+      <c r="Y104" s="28"/>
+      <c r="Z104" s="28"/>
+      <c r="AA104" s="29"/>
     </row>
     <row r="105" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A105" s="25" t="s">
+      <c r="A105" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="B105" s="24"/>
-      <c r="C105" s="24"/>
-      <c r="D105" s="24"/>
-      <c r="E105" s="24"/>
-      <c r="F105" s="24"/>
-      <c r="G105" s="24"/>
-      <c r="H105" s="24"/>
-      <c r="J105" s="24"/>
-      <c r="K105" s="24"/>
-      <c r="L105" s="24"/>
-      <c r="M105" s="24"/>
-      <c r="N105" s="24"/>
-      <c r="O105" s="29"/>
-      <c r="P105" s="29"/>
-      <c r="Q105" s="29"/>
-      <c r="R105" s="29"/>
-      <c r="S105" s="29"/>
-      <c r="T105" s="29"/>
-      <c r="U105" s="29"/>
-      <c r="V105" s="29"/>
-      <c r="W105" s="29"/>
-      <c r="X105" s="31"/>
-      <c r="Y105" s="31"/>
-      <c r="Z105" s="31"/>
-      <c r="AA105" s="32"/>
+      <c r="B105" s="21"/>
+      <c r="C105" s="21"/>
+      <c r="D105" s="21"/>
+      <c r="E105" s="21"/>
+      <c r="F105" s="21"/>
+      <c r="G105" s="21"/>
+      <c r="H105" s="21"/>
+      <c r="J105" s="21"/>
+      <c r="K105" s="21"/>
+      <c r="L105" s="21"/>
+      <c r="M105" s="21"/>
+      <c r="N105" s="21"/>
+      <c r="O105" s="26"/>
+      <c r="P105" s="26"/>
+      <c r="Q105" s="26"/>
+      <c r="R105" s="26"/>
+      <c r="S105" s="26"/>
+      <c r="T105" s="26"/>
+      <c r="U105" s="26"/>
+      <c r="V105" s="26"/>
+      <c r="W105" s="26"/>
+      <c r="X105" s="28"/>
+      <c r="Y105" s="28"/>
+      <c r="Z105" s="28"/>
+      <c r="AA105" s="29"/>
     </row>
     <row r="106" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A106" s="25" t="s">
+      <c r="A106" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="B106" s="24"/>
-      <c r="C106" s="24"/>
-      <c r="D106" s="24"/>
-      <c r="E106" s="24"/>
-      <c r="F106" s="24"/>
-      <c r="G106" s="24"/>
-      <c r="H106" s="24"/>
-      <c r="J106" s="24"/>
-      <c r="K106" s="24"/>
-      <c r="L106" s="24"/>
-      <c r="M106" s="24"/>
-      <c r="N106" s="29"/>
-      <c r="O106" s="29"/>
-      <c r="P106" s="29"/>
-      <c r="Q106" s="29"/>
-      <c r="R106" s="29"/>
-      <c r="S106" s="29"/>
-      <c r="T106" s="29"/>
-      <c r="U106" s="29"/>
-      <c r="V106" s="29"/>
-      <c r="W106" s="29"/>
-      <c r="X106" s="31"/>
-      <c r="Y106" s="31"/>
-      <c r="Z106" s="31"/>
-      <c r="AA106" s="32"/>
+      <c r="B106" s="21"/>
+      <c r="C106" s="21"/>
+      <c r="D106" s="21"/>
+      <c r="E106" s="21"/>
+      <c r="F106" s="21"/>
+      <c r="G106" s="21"/>
+      <c r="H106" s="21"/>
+      <c r="J106" s="21"/>
+      <c r="K106" s="21"/>
+      <c r="L106" s="21"/>
+      <c r="M106" s="21"/>
+      <c r="N106" s="26"/>
+      <c r="O106" s="26"/>
+      <c r="P106" s="26"/>
+      <c r="Q106" s="26"/>
+      <c r="R106" s="26"/>
+      <c r="S106" s="26"/>
+      <c r="T106" s="26"/>
+      <c r="U106" s="26"/>
+      <c r="V106" s="26"/>
+      <c r="W106" s="26"/>
+      <c r="X106" s="28"/>
+      <c r="Y106" s="28"/>
+      <c r="Z106" s="28"/>
+      <c r="AA106" s="29"/>
     </row>
     <row r="107" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A107" s="25" t="s">
+      <c r="A107" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="B107" s="24"/>
-      <c r="C107" s="24"/>
-      <c r="D107" s="24"/>
-      <c r="E107" s="24"/>
-      <c r="F107" s="24"/>
-      <c r="G107" s="24"/>
-      <c r="H107" s="24"/>
-      <c r="J107" s="24"/>
-      <c r="K107" s="24"/>
-      <c r="L107" s="24"/>
-      <c r="M107" s="29"/>
-      <c r="N107" s="29"/>
-      <c r="O107" s="29"/>
-      <c r="P107" s="29"/>
-      <c r="Q107" s="29"/>
-      <c r="R107" s="29"/>
-      <c r="S107" s="29"/>
-      <c r="T107" s="29"/>
-      <c r="U107" s="29"/>
-      <c r="V107" s="29"/>
-      <c r="W107" s="29"/>
-      <c r="X107" s="31"/>
-      <c r="Y107" s="31"/>
-      <c r="Z107" s="31"/>
-      <c r="AA107" s="32"/>
+      <c r="B107" s="21"/>
+      <c r="C107" s="21"/>
+      <c r="D107" s="21"/>
+      <c r="E107" s="21"/>
+      <c r="F107" s="21"/>
+      <c r="G107" s="21"/>
+      <c r="H107" s="21"/>
+      <c r="J107" s="21"/>
+      <c r="K107" s="21"/>
+      <c r="L107" s="21"/>
+      <c r="M107" s="26"/>
+      <c r="N107" s="26"/>
+      <c r="O107" s="26"/>
+      <c r="P107" s="26"/>
+      <c r="Q107" s="26"/>
+      <c r="R107" s="26"/>
+      <c r="S107" s="26"/>
+      <c r="T107" s="26"/>
+      <c r="U107" s="26"/>
+      <c r="V107" s="26"/>
+      <c r="W107" s="26"/>
+      <c r="X107" s="28"/>
+      <c r="Y107" s="28"/>
+      <c r="Z107" s="28"/>
+      <c r="AA107" s="29"/>
     </row>
     <row r="108" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A108" s="25" t="s">
+      <c r="A108" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="B108" s="24"/>
-      <c r="C108" s="24"/>
-      <c r="D108" s="24"/>
-      <c r="E108" s="24"/>
-      <c r="F108" s="24"/>
-      <c r="G108" s="24"/>
-      <c r="H108" s="24"/>
-      <c r="J108" s="24"/>
-      <c r="K108" s="24"/>
-      <c r="L108" s="29"/>
-      <c r="M108" s="29"/>
-      <c r="N108" s="29"/>
-      <c r="O108" s="29"/>
-      <c r="P108" s="29"/>
-      <c r="Q108" s="29"/>
-      <c r="R108" s="29"/>
-      <c r="S108" s="29"/>
-      <c r="T108" s="29"/>
-      <c r="U108" s="29"/>
-      <c r="V108" s="29"/>
-      <c r="W108" s="29"/>
-      <c r="X108" s="31"/>
-      <c r="Y108" s="31"/>
-      <c r="Z108" s="31"/>
-      <c r="AA108" s="32"/>
+      <c r="B108" s="21"/>
+      <c r="C108" s="21"/>
+      <c r="D108" s="21"/>
+      <c r="E108" s="21"/>
+      <c r="F108" s="21"/>
+      <c r="G108" s="21"/>
+      <c r="H108" s="21"/>
+      <c r="J108" s="21"/>
+      <c r="K108" s="21"/>
+      <c r="L108" s="26"/>
+      <c r="M108" s="26"/>
+      <c r="N108" s="26"/>
+      <c r="O108" s="26"/>
+      <c r="P108" s="26"/>
+      <c r="Q108" s="26"/>
+      <c r="R108" s="26"/>
+      <c r="S108" s="26"/>
+      <c r="T108" s="26"/>
+      <c r="U108" s="26"/>
+      <c r="V108" s="26"/>
+      <c r="W108" s="26"/>
+      <c r="X108" s="28"/>
+      <c r="Y108" s="28"/>
+      <c r="Z108" s="28"/>
+      <c r="AA108" s="29"/>
     </row>
     <row r="109" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A109" s="25" t="s">
+      <c r="A109" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="B109" s="24"/>
-      <c r="C109" s="24"/>
-      <c r="D109" s="24"/>
-      <c r="E109" s="24"/>
-      <c r="F109" s="24"/>
-      <c r="G109" s="24"/>
-      <c r="H109" s="24"/>
-      <c r="J109" s="24"/>
-      <c r="K109" s="29"/>
-      <c r="L109" s="29"/>
-      <c r="M109" s="29"/>
-      <c r="N109" s="29"/>
-      <c r="O109" s="29"/>
-      <c r="P109" s="29"/>
-      <c r="Q109" s="29"/>
-      <c r="R109" s="29"/>
-      <c r="S109" s="29"/>
-      <c r="T109" s="29"/>
-      <c r="U109" s="29"/>
-      <c r="V109" s="29"/>
-      <c r="W109" s="29"/>
-      <c r="X109" s="31"/>
-      <c r="Y109" s="31"/>
-      <c r="Z109" s="31"/>
-      <c r="AA109" s="32"/>
+      <c r="B109" s="21"/>
+      <c r="C109" s="21"/>
+      <c r="D109" s="21"/>
+      <c r="E109" s="21"/>
+      <c r="F109" s="21"/>
+      <c r="G109" s="21"/>
+      <c r="H109" s="21"/>
+      <c r="J109" s="21"/>
+      <c r="K109" s="26"/>
+      <c r="L109" s="26"/>
+      <c r="M109" s="26"/>
+      <c r="N109" s="26"/>
+      <c r="O109" s="26"/>
+      <c r="P109" s="26"/>
+      <c r="Q109" s="26"/>
+      <c r="R109" s="26"/>
+      <c r="S109" s="26"/>
+      <c r="T109" s="26"/>
+      <c r="U109" s="26"/>
+      <c r="V109" s="26"/>
+      <c r="W109" s="26"/>
+      <c r="X109" s="28"/>
+      <c r="Y109" s="28"/>
+      <c r="Z109" s="28"/>
+      <c r="AA109" s="29"/>
     </row>
     <row r="110" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A110" s="25" t="s">
+      <c r="A110" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="B110" s="24"/>
-      <c r="C110" s="24"/>
-      <c r="D110" s="24"/>
-      <c r="E110" s="24"/>
-      <c r="F110" s="24"/>
-      <c r="G110" s="24"/>
-      <c r="H110" s="24"/>
-      <c r="J110" s="29"/>
-      <c r="K110" s="29"/>
-      <c r="L110" s="29"/>
-      <c r="M110" s="29"/>
-      <c r="N110" s="29"/>
-      <c r="O110" s="29"/>
-      <c r="P110" s="29"/>
-      <c r="Q110" s="29"/>
-      <c r="R110" s="29"/>
-      <c r="S110" s="29"/>
-      <c r="T110" s="29"/>
-      <c r="U110" s="29"/>
-      <c r="V110" s="29"/>
-      <c r="W110" s="29"/>
-      <c r="X110" s="31"/>
-      <c r="Y110" s="31"/>
-      <c r="Z110" s="31"/>
-      <c r="AA110" s="32"/>
+      <c r="B110" s="21"/>
+      <c r="C110" s="21"/>
+      <c r="D110" s="21"/>
+      <c r="E110" s="21"/>
+      <c r="F110" s="21"/>
+      <c r="G110" s="21"/>
+      <c r="H110" s="21"/>
+      <c r="J110" s="26"/>
+      <c r="K110" s="26"/>
+      <c r="L110" s="26"/>
+      <c r="M110" s="26"/>
+      <c r="N110" s="26"/>
+      <c r="O110" s="26"/>
+      <c r="P110" s="26"/>
+      <c r="Q110" s="26"/>
+      <c r="R110" s="26"/>
+      <c r="S110" s="26"/>
+      <c r="T110" s="26"/>
+      <c r="U110" s="26"/>
+      <c r="V110" s="26"/>
+      <c r="W110" s="26"/>
+      <c r="X110" s="28"/>
+      <c r="Y110" s="28"/>
+      <c r="Z110" s="28"/>
+      <c r="AA110" s="29"/>
     </row>
     <row r="111" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A111" s="25" t="s">
+      <c r="A111" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="B111" s="24"/>
-      <c r="C111" s="24"/>
-      <c r="D111" s="24"/>
-      <c r="E111" s="24"/>
-      <c r="F111" s="24"/>
-      <c r="G111" s="24"/>
-      <c r="H111" s="24"/>
-      <c r="I111" s="29"/>
-      <c r="J111" s="29"/>
-      <c r="K111" s="29"/>
-      <c r="L111" s="29"/>
-      <c r="M111" s="29"/>
-      <c r="N111" s="29"/>
-      <c r="O111" s="29"/>
-      <c r="P111" s="29"/>
-      <c r="Q111" s="29"/>
-      <c r="R111" s="29"/>
-      <c r="S111" s="29"/>
-      <c r="T111" s="29"/>
-      <c r="U111" s="29"/>
-      <c r="V111" s="29"/>
-      <c r="W111" s="29"/>
-      <c r="X111" s="31"/>
-      <c r="Y111" s="31"/>
-      <c r="Z111" s="31"/>
-      <c r="AA111" s="32"/>
+      <c r="B111" s="21"/>
+      <c r="C111" s="21"/>
+      <c r="D111" s="21"/>
+      <c r="E111" s="21"/>
+      <c r="F111" s="21"/>
+      <c r="G111" s="21"/>
+      <c r="H111" s="21"/>
+      <c r="I111" s="26"/>
+      <c r="J111" s="26"/>
+      <c r="K111" s="26"/>
+      <c r="L111" s="26"/>
+      <c r="M111" s="26"/>
+      <c r="N111" s="26"/>
+      <c r="O111" s="26"/>
+      <c r="P111" s="26"/>
+      <c r="Q111" s="26"/>
+      <c r="R111" s="26"/>
+      <c r="S111" s="26"/>
+      <c r="T111" s="26"/>
+      <c r="U111" s="26"/>
+      <c r="V111" s="26"/>
+      <c r="W111" s="26"/>
+      <c r="X111" s="28"/>
+      <c r="Y111" s="28"/>
+      <c r="Z111" s="28"/>
+      <c r="AA111" s="29"/>
     </row>
     <row r="112" spans="1:27" ht="30" x14ac:dyDescent="0.25">
-      <c r="A112" s="25" t="s">
+      <c r="A112" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="B112" s="24"/>
-      <c r="C112" s="24"/>
-      <c r="D112" s="24"/>
-      <c r="E112" s="24"/>
-      <c r="F112" s="24"/>
-      <c r="G112" s="24"/>
-      <c r="H112" s="29"/>
-      <c r="I112" s="29"/>
-      <c r="J112" s="29"/>
-      <c r="K112" s="29"/>
-      <c r="L112" s="29"/>
-      <c r="M112" s="29"/>
-      <c r="N112" s="29"/>
-      <c r="O112" s="29"/>
-      <c r="P112" s="29"/>
-      <c r="Q112" s="29"/>
-      <c r="R112" s="29"/>
-      <c r="S112" s="29"/>
-      <c r="T112" s="29"/>
-      <c r="U112" s="29"/>
-      <c r="V112" s="29"/>
-      <c r="W112" s="29"/>
-      <c r="X112" s="31"/>
-      <c r="Y112" s="31"/>
-      <c r="Z112" s="31"/>
-      <c r="AA112" s="32"/>
+      <c r="B112" s="21"/>
+      <c r="C112" s="21"/>
+      <c r="D112" s="21"/>
+      <c r="E112" s="21"/>
+      <c r="F112" s="21"/>
+      <c r="G112" s="21"/>
+      <c r="H112" s="26"/>
+      <c r="I112" s="26"/>
+      <c r="J112" s="26"/>
+      <c r="K112" s="26"/>
+      <c r="L112" s="26"/>
+      <c r="M112" s="26"/>
+      <c r="N112" s="26"/>
+      <c r="O112" s="26"/>
+      <c r="P112" s="26"/>
+      <c r="Q112" s="26"/>
+      <c r="R112" s="26"/>
+      <c r="S112" s="26"/>
+      <c r="T112" s="26"/>
+      <c r="U112" s="26"/>
+      <c r="V112" s="26"/>
+      <c r="W112" s="26"/>
+      <c r="X112" s="28"/>
+      <c r="Y112" s="28"/>
+      <c r="Z112" s="28"/>
+      <c r="AA112" s="29"/>
     </row>
     <row r="113" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A113" s="25" t="s">
+      <c r="A113" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="B113" s="24"/>
-      <c r="C113" s="24"/>
-      <c r="D113" s="24"/>
-      <c r="E113" s="24"/>
-      <c r="F113" s="24"/>
-      <c r="G113" s="29"/>
-      <c r="H113" s="29"/>
-      <c r="I113" s="29"/>
-      <c r="J113" s="29"/>
-      <c r="K113" s="29"/>
-      <c r="L113" s="29"/>
-      <c r="M113" s="29"/>
-      <c r="N113" s="29"/>
-      <c r="O113" s="29"/>
-      <c r="P113" s="29"/>
-      <c r="Q113" s="29"/>
-      <c r="R113" s="29"/>
-      <c r="S113" s="29"/>
-      <c r="T113" s="29"/>
-      <c r="U113" s="29"/>
-      <c r="V113" s="29"/>
-      <c r="W113" s="29"/>
-      <c r="X113" s="31"/>
-      <c r="Y113" s="31"/>
-      <c r="Z113" s="31"/>
-      <c r="AA113" s="32"/>
+      <c r="B113" s="21"/>
+      <c r="C113" s="21"/>
+      <c r="D113" s="21"/>
+      <c r="E113" s="21"/>
+      <c r="F113" s="21"/>
+      <c r="G113" s="26"/>
+      <c r="H113" s="26"/>
+      <c r="I113" s="26"/>
+      <c r="J113" s="26"/>
+      <c r="K113" s="26"/>
+      <c r="L113" s="26"/>
+      <c r="M113" s="26"/>
+      <c r="N113" s="26"/>
+      <c r="O113" s="26"/>
+      <c r="P113" s="26"/>
+      <c r="Q113" s="26"/>
+      <c r="R113" s="26"/>
+      <c r="S113" s="26"/>
+      <c r="T113" s="26"/>
+      <c r="U113" s="26"/>
+      <c r="V113" s="26"/>
+      <c r="W113" s="26"/>
+      <c r="X113" s="28"/>
+      <c r="Y113" s="28"/>
+      <c r="Z113" s="28"/>
+      <c r="AA113" s="29"/>
     </row>
     <row r="114" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B114" s="24"/>
-      <c r="C114" s="24"/>
-      <c r="D114" s="24"/>
-      <c r="E114" s="24"/>
-      <c r="F114" s="29"/>
-      <c r="G114" s="29"/>
-      <c r="H114" s="29"/>
-      <c r="I114" s="29"/>
-      <c r="J114" s="29"/>
-      <c r="K114" s="29"/>
-      <c r="L114" s="29"/>
-      <c r="M114" s="29"/>
-      <c r="N114" s="29"/>
-      <c r="O114" s="29"/>
-      <c r="P114" s="29"/>
-      <c r="Q114" s="29"/>
-      <c r="R114" s="29"/>
-      <c r="S114" s="29"/>
-      <c r="T114" s="29"/>
-      <c r="U114" s="29"/>
-      <c r="V114" s="29"/>
-      <c r="W114" s="29"/>
-      <c r="X114" s="31"/>
-      <c r="Y114" s="31"/>
-      <c r="Z114" s="31"/>
-      <c r="AA114" s="32"/>
+      <c r="B114" s="21"/>
+      <c r="C114" s="21"/>
+      <c r="D114" s="21"/>
+      <c r="E114" s="21"/>
+      <c r="F114" s="26"/>
+      <c r="G114" s="26"/>
+      <c r="H114" s="26"/>
+      <c r="I114" s="26"/>
+      <c r="J114" s="26"/>
+      <c r="K114" s="26"/>
+      <c r="L114" s="26"/>
+      <c r="M114" s="26"/>
+      <c r="N114" s="26"/>
+      <c r="O114" s="26"/>
+      <c r="P114" s="26"/>
+      <c r="Q114" s="26"/>
+      <c r="R114" s="26"/>
+      <c r="S114" s="26"/>
+      <c r="T114" s="26"/>
+      <c r="U114" s="26"/>
+      <c r="V114" s="26"/>
+      <c r="W114" s="26"/>
+      <c r="X114" s="28"/>
+      <c r="Y114" s="28"/>
+      <c r="Z114" s="28"/>
+      <c r="AA114" s="29"/>
     </row>
     <row r="115" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B115" s="29"/>
-      <c r="C115" s="29"/>
-      <c r="D115" s="29"/>
-      <c r="E115" s="29"/>
-      <c r="F115" s="29"/>
-      <c r="G115" s="29"/>
-      <c r="H115" s="29"/>
-      <c r="I115" s="29"/>
-      <c r="J115" s="29"/>
-      <c r="K115" s="29"/>
-      <c r="L115" s="29"/>
-      <c r="M115" s="29"/>
-      <c r="N115" s="29"/>
-      <c r="O115" s="29"/>
-      <c r="P115" s="29"/>
-      <c r="Q115" s="29"/>
-      <c r="R115" s="29"/>
-      <c r="S115" s="29"/>
-      <c r="T115" s="29"/>
-      <c r="U115" s="29"/>
-      <c r="V115" s="29"/>
-      <c r="W115" s="29"/>
-      <c r="X115" s="31"/>
-      <c r="Y115" s="31"/>
-      <c r="Z115" s="31"/>
-      <c r="AA115" s="32"/>
+      <c r="B115" s="26"/>
+      <c r="C115" s="26"/>
+      <c r="D115" s="26"/>
+      <c r="E115" s="26"/>
+      <c r="F115" s="26"/>
+      <c r="G115" s="26"/>
+      <c r="H115" s="26"/>
+      <c r="I115" s="26"/>
+      <c r="J115" s="26"/>
+      <c r="K115" s="26"/>
+      <c r="L115" s="26"/>
+      <c r="M115" s="26"/>
+      <c r="N115" s="26"/>
+      <c r="O115" s="26"/>
+      <c r="P115" s="26"/>
+      <c r="Q115" s="26"/>
+      <c r="R115" s="26"/>
+      <c r="S115" s="26"/>
+      <c r="T115" s="26"/>
+      <c r="U115" s="26"/>
+      <c r="V115" s="26"/>
+      <c r="W115" s="26"/>
+      <c r="X115" s="28"/>
+      <c r="Y115" s="28"/>
+      <c r="Z115" s="28"/>
+      <c r="AA115" s="29"/>
     </row>
     <row r="116" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B116" s="29"/>
-      <c r="C116" s="29"/>
-      <c r="D116" s="29"/>
-      <c r="E116" s="29"/>
-      <c r="F116" s="29"/>
-      <c r="G116" s="29"/>
-      <c r="H116" s="29"/>
-      <c r="I116" s="29"/>
-      <c r="J116" s="29"/>
-      <c r="K116" s="29"/>
-      <c r="L116" s="29"/>
-      <c r="M116" s="29"/>
-      <c r="N116" s="29"/>
-      <c r="O116" s="29"/>
-      <c r="P116" s="29"/>
-      <c r="Q116" s="29"/>
-      <c r="R116" s="29"/>
-      <c r="S116" s="29"/>
-      <c r="T116" s="29"/>
-      <c r="U116" s="29"/>
-      <c r="V116" s="29"/>
-      <c r="W116" s="29"/>
-      <c r="X116" s="31"/>
-      <c r="Y116" s="31"/>
-      <c r="Z116" s="31"/>
-      <c r="AA116" s="32"/>
+      <c r="B116" s="26"/>
+      <c r="C116" s="26"/>
+      <c r="D116" s="26"/>
+      <c r="E116" s="26"/>
+      <c r="F116" s="26"/>
+      <c r="G116" s="26"/>
+      <c r="H116" s="26"/>
+      <c r="I116" s="26"/>
+      <c r="J116" s="26"/>
+      <c r="K116" s="26"/>
+      <c r="L116" s="26"/>
+      <c r="M116" s="26"/>
+      <c r="N116" s="26"/>
+      <c r="O116" s="26"/>
+      <c r="P116" s="26"/>
+      <c r="Q116" s="26"/>
+      <c r="R116" s="26"/>
+      <c r="S116" s="26"/>
+      <c r="T116" s="26"/>
+      <c r="U116" s="26"/>
+      <c r="V116" s="26"/>
+      <c r="W116" s="26"/>
+      <c r="X116" s="28"/>
+      <c r="Y116" s="28"/>
+      <c r="Z116" s="28"/>
+      <c r="AA116" s="29"/>
     </row>
     <row r="117" spans="1:27" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="33" t="s">
+      <c r="A117" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="B117" s="29"/>
-      <c r="C117" s="29"/>
-      <c r="D117" s="29"/>
-      <c r="E117" s="29"/>
-      <c r="F117" s="29"/>
-      <c r="G117" s="29"/>
-      <c r="H117" s="29"/>
-      <c r="I117" s="29"/>
-      <c r="J117" s="29"/>
-      <c r="K117" s="29"/>
-      <c r="L117" s="29"/>
-      <c r="M117" s="29"/>
-      <c r="N117" s="29"/>
-      <c r="O117" s="29"/>
-      <c r="P117" s="29"/>
-      <c r="Q117" s="29"/>
-      <c r="R117" s="29"/>
-      <c r="S117" s="29"/>
-      <c r="T117" s="29"/>
-      <c r="U117" s="29"/>
-      <c r="V117" s="29"/>
-      <c r="W117" s="29"/>
-      <c r="X117" s="31"/>
-      <c r="Y117" s="31"/>
-      <c r="Z117" s="31"/>
-      <c r="AA117" s="32"/>
+      <c r="B117" s="26"/>
+      <c r="C117" s="26"/>
+      <c r="D117" s="26"/>
+      <c r="E117" s="26"/>
+      <c r="F117" s="26"/>
+      <c r="G117" s="26"/>
+      <c r="H117" s="26"/>
+      <c r="I117" s="26"/>
+      <c r="J117" s="26"/>
+      <c r="K117" s="26"/>
+      <c r="L117" s="26"/>
+      <c r="M117" s="26"/>
+      <c r="N117" s="26"/>
+      <c r="O117" s="26"/>
+      <c r="P117" s="26"/>
+      <c r="Q117" s="26"/>
+      <c r="R117" s="26"/>
+      <c r="S117" s="26"/>
+      <c r="T117" s="26"/>
+      <c r="U117" s="26"/>
+      <c r="V117" s="26"/>
+      <c r="W117" s="26"/>
+      <c r="X117" s="28"/>
+      <c r="Y117" s="28"/>
+      <c r="Z117" s="28"/>
+      <c r="AA117" s="29"/>
     </row>
     <row r="118" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A118" s="26" t="s">
+      <c r="A118" s="23" t="s">
         <v>147</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Upgraded some cells to drop down boxes for easy selection.
</commit_message>
<xml_diff>
--- a/SampleTestData.xlsx
+++ b/SampleTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Manage Performance" sheetId="13" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="202">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1184,7 +1184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FU3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
@@ -2948,9 +2948,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:EX21"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T24" sqref="T24"/>
+      <selection pane="bottomLeft" activeCell="AD21" sqref="AD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5862,18 +5862,6 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Fields!$A$11:$M$11</xm:f>
-          </x14:formula1>
-          <xm:sqref>H3:H15</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Fields!$A$11:$R$11</xm:f>
-          </x14:formula1>
-          <xm:sqref>H16:H20</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
             <xm:f>Fields!$C$14:$P$14</xm:f>
           </x14:formula1>
           <xm:sqref>J16 L16 N16 P16 R16 T16 V16 X16 Z16 AB16 AD16 AF16 AH16 AJ16</xm:sqref>
@@ -5896,6 +5884,18 @@
           </x14:formula1>
           <xm:sqref>J20 L20 N20 P20 R20 T20 V20 X20 Z20 AB20 AD20 AF20 AH20 AJ20</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Fields!$A$11:$S$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>H21 H15 H14 H13 H12 H11 H10 H9 H8 H7 H6 H5 H4 H3 H20 H19 H18 H17 H16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Fields!$C$19:$M$19</xm:f>
+          </x14:formula1>
+          <xm:sqref>J21 L21 N21 P21 R21 T21 V21 X21 Z21 AB21 AD21</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -5907,8 +5907,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AE118"/>
   <sheetViews>
-    <sheetView topLeftCell="M7" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="J7" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6446,6 +6446,9 @@
       <c r="R11" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="S11" s="14" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
@@ -6698,6 +6701,39 @@
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>27</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L19" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="M19" s="14" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated the Configuration File
</commit_message>
<xml_diff>
--- a/SampleTestData.xlsx
+++ b/SampleTestData.xlsx
@@ -5,26 +5,30 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerrick.m.falogme\Desktop\my_workspace\HCM-Configs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john.lester.f.lucena\Desktop\HCM POC\Repositories\Configurations\HCM_Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Configure Offerings" sheetId="11" r:id="rId1"/>
-    <sheet name="Compensation Management" sheetId="9" r:id="rId2"/>
-    <sheet name="Manage Performance" sheetId="7" r:id="rId3"/>
+    <sheet name="ManageWorkerGoalSetting" sheetId="12" r:id="rId2"/>
+    <sheet name="ManageWorkerGoalSettingValidate" sheetId="13" r:id="rId3"/>
+    <sheet name="Compensation Management" sheetId="9" r:id="rId4"/>
+    <sheet name="Manage Performance" sheetId="7" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="Location">'[1]Optional Lists'!$F$9:$F$1815</definedName>
+    <definedName name="MainTaskFolder">[2]ManageWorkerGoalSettingLookups!$A$2:$A$4</definedName>
     <definedName name="SetID">'[1]Optional Lists'!$E$9:$E$19</definedName>
     <definedName name="Status">'[1]Optional Lists'!$A$33:$A$34</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="73">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -135,142 +139,7 @@
     <t>Workforce Profiles</t>
   </si>
   <si>
-    <t>Test Case 12</t>
-  </si>
-  <si>
-    <t>Project Integration Gateway</t>
-  </si>
-  <si>
-    <t>Capital Projects</t>
-  </si>
-  <si>
-    <t>Internal Project Billing</t>
-  </si>
-  <si>
-    <t>Project Performance Reporting</t>
-  </si>
-  <si>
-    <t>Product Management</t>
-  </si>
-  <si>
-    <t>Leads Business Intelligence Analytics</t>
-  </si>
-  <si>
-    <t>Opportunity Landscape Business Intelligence Analytics</t>
-  </si>
-  <si>
     <t>Human Resources Business Intelligence Analytics</t>
-  </si>
-  <si>
-    <t>Supplier Portal</t>
-  </si>
-  <si>
-    <t>Item and Catalog Management</t>
-  </si>
-  <si>
-    <t>Inventory Organizations</t>
-  </si>
-  <si>
-    <t>Catalogs</t>
-  </si>
-  <si>
-    <t>Structures</t>
-  </si>
-  <si>
-    <t>Suppliers for Product Management</t>
-  </si>
-  <si>
-    <t>Item Mass Update</t>
-  </si>
-  <si>
-    <t>Data Governance</t>
-  </si>
-  <si>
-    <t>New Item Requests</t>
-  </si>
-  <si>
-    <t>Change Orders</t>
-  </si>
-  <si>
-    <t>Product Rules</t>
-  </si>
-  <si>
-    <t>Data Quality Rules for Products</t>
-  </si>
-  <si>
-    <t>Audit Trail</t>
-  </si>
-  <si>
-    <t>Data Consolidation</t>
-  </si>
-  <si>
-    <t>Product Spoke Systems</t>
-  </si>
-  <si>
-    <t>Item Batches</t>
-  </si>
-  <si>
-    <t>Data Pool Integration</t>
-  </si>
-  <si>
-    <t>Data Quality for Products</t>
-  </si>
-  <si>
-    <t>Supplier Collaboration</t>
-  </si>
-  <si>
-    <t>Configurator</t>
-  </si>
-  <si>
-    <t>Configurator Modeling Environment</t>
-  </si>
-  <si>
-    <t>Product Development</t>
-  </si>
-  <si>
-    <t>Sales Prediction Engine Business Intelligence Analytics</t>
-  </si>
-  <si>
-    <t>Transaction Tax</t>
-  </si>
-  <si>
-    <t>Product Development Configuration</t>
-  </si>
-  <si>
-    <t>Project Execution Management</t>
-  </si>
-  <si>
-    <t>Project Financial Management</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>Supply Chain Financial Orchestration</t>
-  </si>
-  <si>
-    <t>Supply Chain Managerial Accounting</t>
-  </si>
-  <si>
-    <t>Test Case 13</t>
-  </si>
-  <si>
-    <t>Test Case 14</t>
-  </si>
-  <si>
-    <t>Test Case 15</t>
-  </si>
-  <si>
-    <t>Test Case 16</t>
-  </si>
-  <si>
-    <t>Test Case 17</t>
-  </si>
-  <si>
-    <t>Test Case 18</t>
-  </si>
-  <si>
-    <t>Test Case 19</t>
   </si>
   <si>
     <t>Worker Goal Setting</t>
@@ -309,121 +178,85 @@
     <t>Workforce Management</t>
   </si>
   <si>
-    <t>Receipt Accounting</t>
-  </si>
-  <si>
-    <t>Cost Accounting</t>
-  </si>
-  <si>
-    <t>Cost and Profit Planning</t>
-  </si>
-  <si>
-    <t>Sales Prediction Engine</t>
-  </si>
-  <si>
-    <t>Outlook Integration</t>
-  </si>
-  <si>
-    <t>Quotas</t>
-  </si>
-  <si>
-    <t>References</t>
-  </si>
-  <si>
-    <t>Competitors</t>
-  </si>
-  <si>
-    <t>Sales Forecasting</t>
-  </si>
-  <si>
-    <t>Partners</t>
-  </si>
-  <si>
-    <t>Partner Business Intelligence Analytics</t>
-  </si>
-  <si>
-    <t>Partner Performance</t>
-  </si>
-  <si>
-    <t>Partner Deals</t>
-  </si>
-  <si>
-    <t>Partner Programs</t>
-  </si>
-  <si>
-    <t>Territory Management</t>
-  </si>
-  <si>
-    <t>Sales Business Intelligence Analytics</t>
-  </si>
-  <si>
-    <t>Quota Management Business Intelligence Analytics</t>
-  </si>
-  <si>
-    <t>Territory Management Business Intelligence Analytics</t>
-  </si>
-  <si>
-    <t>Opportunity and Revenue Management Business Intelligence Analytics</t>
-  </si>
-  <si>
-    <t>Customer Interactions Management</t>
-  </si>
-  <si>
-    <t>Sales Forecasting Management Business Intelligence Analytics</t>
-  </si>
-  <si>
-    <t>Basic Catalogs</t>
-  </si>
-  <si>
-    <t>Sales Cloud Integration</t>
-  </si>
-  <si>
-    <t>Project Resource Management</t>
-  </si>
-  <si>
-    <t>Burdening</t>
-  </si>
-  <si>
-    <t>Project Control</t>
-  </si>
-  <si>
-    <t>Project Costing</t>
-  </si>
-  <si>
-    <t>Project Billing</t>
-  </si>
-  <si>
-    <t>Project Business Intelligence Analytics</t>
-  </si>
-  <si>
-    <t>Project Revenue and Billing Business Intelligence Analytics</t>
-  </si>
-  <si>
-    <t>Project Performance Business Intelligence Analytics</t>
-  </si>
-  <si>
-    <t>Project Control and Costing Business Intelligence Analytics</t>
-  </si>
-  <si>
-    <t>Product Requirements and Ideation Management</t>
-  </si>
-  <si>
-    <t>Concept Design Management</t>
-  </si>
-  <si>
-    <t>Product Lifecycle Portfolio Management</t>
-  </si>
-  <si>
-    <t>Product Management Business Intelligence Analytics</t>
-  </si>
-  <si>
-    <t>Advanced Catalogs</t>
-  </si>
-  <si>
     <t>In Progress</t>
   </si>
   <si>
     <t>Implemented</t>
+  </si>
+  <si>
+    <t>Test Case 2</t>
+  </si>
+  <si>
+    <t>Test Case 3</t>
+  </si>
+  <si>
+    <t>Total Compensation Statements</t>
+  </si>
+  <si>
+    <t>13 ~ 18</t>
+  </si>
+  <si>
+    <t>Task Folder</t>
+  </si>
+  <si>
+    <t>Task Folder Items: L2</t>
+  </si>
+  <si>
+    <t>Task Folder Items : L3</t>
+  </si>
+  <si>
+    <t>Task Folder Items: L4</t>
+  </si>
+  <si>
+    <t>Setting Lookups</t>
+  </si>
+  <si>
+    <t>Lookup Code</t>
+  </si>
+  <si>
+    <t>Display Sequence</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Meaning</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Manage Worker Goal Setting Lookups</t>
+  </si>
+  <si>
+    <t>HRG_DEV_GOAL_CATEGORY</t>
+  </si>
+  <si>
+    <t>01/01/0001</t>
+  </si>
+  <si>
+    <t>This is for testing purpose.</t>
+  </si>
+  <si>
+    <t>DevOps_TEST_TERM_1</t>
+  </si>
+  <si>
+    <t>DevOps v0_001</t>
+  </si>
+  <si>
+    <t>Define Worker Goal Setting</t>
+  </si>
+  <si>
+    <t>Goal Name</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Devops-Demo</t>
   </si>
 </sst>
 </file>
@@ -481,7 +314,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -588,12 +421,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -653,6 +521,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -9838,6 +9724,43 @@
         <row r="1815">
           <cell r="F1815" t="str">
             <v/>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Configure Offerings"/>
+      <sheetName val="Compensation Management"/>
+      <sheetName val="Manage Performance"/>
+      <sheetName val="ManageWorkerGoalSetting"/>
+      <sheetName val="ManageWorkerGoalSettingLookups"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4">
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>Compensation Management</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>Workforce Deployment</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>Workforce Development</v>
           </cell>
         </row>
       </sheetData>
@@ -10109,11 +10032,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FZ10"/>
+  <dimension ref="A1:GA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="F1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10125,93 +10048,93 @@
     <col min="5" max="5" width="79.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="67.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="55.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="54.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="44" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="42" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="49.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="50.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="25" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="15" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="13" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="11.5703125" customWidth="1"/>
-    <col min="59" max="59" width="18.85546875" customWidth="1"/>
-    <col min="60" max="60" width="8.7109375" customWidth="1"/>
-    <col min="61" max="61" width="12.28515625" customWidth="1"/>
-    <col min="62" max="62" width="14.28515625" customWidth="1"/>
-    <col min="63" max="63" width="16.85546875" customWidth="1"/>
-    <col min="64" max="64" width="18.85546875" customWidth="1"/>
-    <col min="65" max="65" width="11.5703125" customWidth="1"/>
-    <col min="66" max="67" width="18.85546875" customWidth="1"/>
-    <col min="68" max="68" width="8.7109375" customWidth="1"/>
-    <col min="69" max="69" width="12.28515625" customWidth="1"/>
-    <col min="70" max="77" width="20.7109375" customWidth="1"/>
-    <col min="78" max="78" width="19.28515625" customWidth="1"/>
-    <col min="79" max="93" width="3" customWidth="1"/>
-    <col min="94" max="100" width="16.42578125" customWidth="1"/>
-    <col min="101" max="101" width="12.42578125" customWidth="1"/>
-    <col min="102" max="102" width="18.42578125" customWidth="1"/>
-    <col min="103" max="103" width="16.140625" customWidth="1"/>
-    <col min="104" max="104" width="15.5703125" customWidth="1"/>
-    <col min="105" max="106" width="14.28515625" customWidth="1"/>
-    <col min="111" max="111" width="18.42578125" customWidth="1"/>
-    <col min="112" max="112" width="14.85546875" customWidth="1"/>
-    <col min="114" max="114" width="11.42578125" customWidth="1"/>
-    <col min="115" max="115" width="12.5703125" customWidth="1"/>
-    <col min="118" max="118" width="11" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="12.7109375" customWidth="1"/>
-    <col min="122" max="122" width="16.85546875" customWidth="1"/>
-    <col min="127" max="127" width="11.42578125" customWidth="1"/>
-    <col min="129" max="129" width="13.42578125" customWidth="1"/>
-    <col min="130" max="130" width="12.5703125" customWidth="1"/>
-    <col min="131" max="131" width="12" customWidth="1"/>
-    <col min="132" max="132" width="10" customWidth="1"/>
-    <col min="138" max="138" width="10.85546875" customWidth="1"/>
-    <col min="139" max="139" width="18.42578125" customWidth="1"/>
+    <col min="8" max="9" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="67.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="50.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="50" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="55.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="54.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="44" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="42" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="25" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="15" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="13" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.5703125" customWidth="1"/>
+    <col min="60" max="60" width="18.85546875" customWidth="1"/>
+    <col min="61" max="61" width="8.7109375" customWidth="1"/>
+    <col min="62" max="62" width="12.28515625" customWidth="1"/>
+    <col min="63" max="63" width="14.28515625" customWidth="1"/>
+    <col min="64" max="64" width="16.85546875" customWidth="1"/>
+    <col min="65" max="65" width="18.85546875" customWidth="1"/>
+    <col min="66" max="66" width="11.5703125" customWidth="1"/>
+    <col min="67" max="68" width="18.85546875" customWidth="1"/>
+    <col min="69" max="69" width="8.7109375" customWidth="1"/>
+    <col min="70" max="70" width="12.28515625" customWidth="1"/>
+    <col min="71" max="78" width="20.7109375" customWidth="1"/>
+    <col min="79" max="79" width="19.28515625" customWidth="1"/>
+    <col min="80" max="94" width="3" customWidth="1"/>
+    <col min="95" max="101" width="16.42578125" customWidth="1"/>
+    <col min="102" max="102" width="12.42578125" customWidth="1"/>
+    <col min="103" max="103" width="18.42578125" customWidth="1"/>
+    <col min="104" max="104" width="16.140625" customWidth="1"/>
+    <col min="105" max="105" width="15.5703125" customWidth="1"/>
+    <col min="106" max="107" width="14.28515625" customWidth="1"/>
+    <col min="112" max="112" width="18.42578125" customWidth="1"/>
+    <col min="113" max="113" width="14.85546875" customWidth="1"/>
+    <col min="115" max="115" width="11.42578125" customWidth="1"/>
+    <col min="116" max="116" width="12.5703125" customWidth="1"/>
+    <col min="119" max="119" width="11" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="12.7109375" customWidth="1"/>
+    <col min="123" max="123" width="16.85546875" customWidth="1"/>
+    <col min="128" max="128" width="11.42578125" customWidth="1"/>
+    <col min="130" max="130" width="13.42578125" customWidth="1"/>
+    <col min="131" max="131" width="12.5703125" customWidth="1"/>
+    <col min="132" max="132" width="12" customWidth="1"/>
+    <col min="133" max="133" width="10" customWidth="1"/>
+    <col min="139" max="139" width="10.85546875" customWidth="1"/>
+    <col min="140" max="140" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:182" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:183" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19">
         <v>0</v>
       </c>
@@ -10237,262 +10160,264 @@
         <v>7</v>
       </c>
       <c r="I1" s="19">
+        <v>8</v>
+      </c>
+      <c r="J1" s="19">
         <v>9</v>
       </c>
-      <c r="J1" s="19">
-        <v>8</v>
-      </c>
       <c r="K1" s="19">
+        <v>10</v>
+      </c>
+      <c r="L1" s="19">
         <v>9</v>
       </c>
-      <c r="L1" s="19">
+      <c r="M1" s="19">
         <v>10</v>
       </c>
-      <c r="M1" s="19">
+      <c r="N1" s="19">
         <v>11</v>
       </c>
-      <c r="N1" s="19">
+      <c r="O1" s="19">
         <v>12</v>
       </c>
-      <c r="O1" s="19">
+      <c r="P1" s="19">
         <v>13</v>
       </c>
-      <c r="P1" s="19">
+      <c r="Q1" s="19">
         <v>14</v>
       </c>
-      <c r="Q1" s="19">
+      <c r="R1" s="19">
         <v>15</v>
       </c>
-      <c r="R1" s="19">
+      <c r="S1" s="19">
         <v>16</v>
       </c>
-      <c r="S1" s="19">
+      <c r="T1" s="19">
         <v>17</v>
       </c>
-      <c r="T1" s="19">
+      <c r="U1" s="19">
         <v>18</v>
       </c>
-      <c r="U1" s="19">
+      <c r="V1" s="19">
         <v>19</v>
       </c>
-      <c r="V1" s="19">
+      <c r="W1" s="19">
         <v>20</v>
       </c>
-      <c r="W1" s="19">
+      <c r="X1" s="19">
         <v>21</v>
       </c>
-      <c r="X1" s="19">
+      <c r="Y1" s="19">
         <v>22</v>
       </c>
-      <c r="Y1" s="19">
+      <c r="Z1" s="19">
         <v>23</v>
       </c>
-      <c r="Z1" s="19">
+      <c r="AA1" s="19">
         <v>24</v>
       </c>
-      <c r="AA1" s="19">
+      <c r="AB1" s="19">
         <v>25</v>
       </c>
-      <c r="AB1" s="19">
+      <c r="AC1" s="19">
         <v>26</v>
       </c>
-      <c r="AC1" s="19">
+      <c r="AD1" s="19">
         <v>27</v>
       </c>
-      <c r="AD1" s="19">
+      <c r="AE1" s="19">
         <v>28</v>
       </c>
-      <c r="AE1" s="19">
+      <c r="AF1" s="19">
         <v>29</v>
       </c>
-      <c r="AF1" s="19">
+      <c r="AG1" s="19">
         <v>30</v>
       </c>
-      <c r="AG1" s="19">
+      <c r="AH1" s="19">
         <v>31</v>
       </c>
-      <c r="AH1" s="19">
+      <c r="AI1" s="19">
         <v>32</v>
       </c>
-      <c r="AI1" s="19">
+      <c r="AJ1" s="19">
         <v>33</v>
       </c>
-      <c r="AJ1" s="19">
+      <c r="AK1" s="19">
         <v>34</v>
       </c>
-      <c r="AK1" s="19">
+      <c r="AL1" s="19">
         <v>35</v>
       </c>
-      <c r="AL1" s="19">
+      <c r="AM1" s="19">
         <v>36</v>
       </c>
-      <c r="AM1" s="19">
+      <c r="AN1" s="19">
         <v>37</v>
       </c>
-      <c r="AN1" s="19">
+      <c r="AO1" s="19">
         <v>38</v>
       </c>
-      <c r="AO1" s="19">
+      <c r="AP1" s="19">
         <v>39</v>
       </c>
-      <c r="AP1" s="19">
+      <c r="AQ1" s="19">
         <v>40</v>
       </c>
-      <c r="AQ1" s="19">
+      <c r="AR1" s="19">
         <v>41</v>
       </c>
-      <c r="AR1" s="19">
+      <c r="AS1" s="19">
         <v>42</v>
       </c>
-      <c r="AS1" s="19">
+      <c r="AT1" s="19">
         <v>43</v>
       </c>
-      <c r="AT1" s="19">
+      <c r="AU1" s="19">
         <v>44</v>
       </c>
-      <c r="AU1" s="19">
+      <c r="AV1" s="19">
         <v>45</v>
       </c>
-      <c r="AV1" s="19">
+      <c r="AW1" s="19">
         <v>46</v>
       </c>
-      <c r="AW1" s="19">
+      <c r="AX1" s="19">
         <v>47</v>
       </c>
-      <c r="AX1" s="19">
+      <c r="AY1" s="19">
         <v>48</v>
       </c>
-      <c r="AY1" s="19">
+      <c r="AZ1" s="19">
         <v>49</v>
       </c>
-      <c r="AZ1" s="19">
+      <c r="BA1" s="19">
         <v>50</v>
       </c>
-      <c r="BA1" s="19">
+      <c r="BB1" s="19">
         <v>51</v>
       </c>
-      <c r="BB1" s="19">
+      <c r="BC1" s="19">
         <v>52</v>
       </c>
-      <c r="BC1" s="19">
+      <c r="BD1" s="19">
         <v>53</v>
       </c>
-      <c r="BD1" s="19">
+      <c r="BE1" s="19">
         <v>54</v>
       </c>
-      <c r="BE1" s="19">
+      <c r="BF1" s="19">
         <v>55</v>
       </c>
-      <c r="BF1" s="19">
+      <c r="BG1" s="19">
         <v>56</v>
       </c>
-      <c r="BG1" s="19">
+      <c r="BH1" s="19">
         <v>57</v>
       </c>
-      <c r="BH1" s="19">
+      <c r="BI1" s="19">
         <v>58</v>
       </c>
-      <c r="BI1" s="19">
+      <c r="BJ1" s="19">
         <v>59</v>
       </c>
-      <c r="BJ1" s="19">
+      <c r="BK1" s="19">
         <v>60</v>
       </c>
-      <c r="BK1" s="19">
+      <c r="BL1" s="19">
         <v>61</v>
       </c>
-      <c r="BL1" s="19">
+      <c r="BM1" s="19">
         <v>62</v>
       </c>
-      <c r="BM1" s="19">
+      <c r="BN1" s="19">
         <v>63</v>
       </c>
-      <c r="BN1" s="19">
+      <c r="BO1" s="19">
         <v>64</v>
       </c>
-      <c r="BO1" s="19">
+      <c r="BP1" s="19">
         <v>65</v>
       </c>
-      <c r="BP1" s="19">
+      <c r="BQ1" s="19">
         <v>66</v>
       </c>
-      <c r="BQ1" s="19">
+      <c r="BR1" s="19">
         <v>67</v>
       </c>
-      <c r="BR1" s="19">
+      <c r="BS1" s="19">
         <v>68</v>
       </c>
-      <c r="BS1" s="19">
+      <c r="BT1" s="19">
         <v>69</v>
       </c>
-      <c r="BT1" s="19">
+      <c r="BU1" s="19">
         <v>70</v>
       </c>
-      <c r="BU1" s="19">
+      <c r="BV1" s="19">
         <v>71</v>
       </c>
-      <c r="BV1" s="19">
+      <c r="BW1" s="19">
         <v>72</v>
       </c>
-      <c r="BW1" s="19">
+      <c r="BX1" s="19">
         <v>73</v>
       </c>
-      <c r="BX1" s="19">
+      <c r="BY1" s="19">
         <v>74</v>
       </c>
-      <c r="BY1" s="19">
+      <c r="BZ1" s="19">
         <v>75</v>
       </c>
-      <c r="BZ1" s="19">
+      <c r="CA1" s="19">
         <v>76</v>
       </c>
-      <c r="CA1" s="19">
+      <c r="CB1" s="19">
         <v>77</v>
       </c>
-      <c r="CB1" s="19">
+      <c r="CC1" s="19">
         <v>78</v>
       </c>
-      <c r="CC1" s="19">
+      <c r="CD1" s="19">
         <v>79</v>
       </c>
-      <c r="CD1" s="19">
+      <c r="CE1" s="19">
         <v>80</v>
       </c>
-      <c r="CE1" s="19">
+      <c r="CF1" s="19">
         <v>81</v>
       </c>
-      <c r="CF1" s="19">
+      <c r="CG1" s="19">
         <v>82</v>
       </c>
-      <c r="CG1" s="19">
+      <c r="CH1" s="19">
         <v>83</v>
       </c>
-      <c r="CH1" s="19">
+      <c r="CI1" s="19">
         <v>84</v>
       </c>
-      <c r="CI1" s="19">
+      <c r="CJ1" s="19">
         <v>85</v>
       </c>
-      <c r="CJ1" s="19">
+      <c r="CK1" s="19">
         <v>86</v>
       </c>
-      <c r="CK1" s="19">
+      <c r="CL1" s="19">
         <v>87</v>
       </c>
-      <c r="CL1" s="19">
+      <c r="CM1" s="19">
         <v>88</v>
       </c>
-      <c r="CM1" s="19">
+      <c r="CN1" s="19">
         <v>89</v>
       </c>
-      <c r="CN1" s="19">
+      <c r="CO1" s="19">
         <v>90</v>
       </c>
-      <c r="CO1" s="19">
+      <c r="CP1" s="19">
         <v>91</v>
       </c>
-      <c r="CP1" s="18"/>
-      <c r="CQ1" s="1"/>
+      <c r="CQ1" s="18"/>
       <c r="CR1" s="1"/>
       <c r="CS1" s="1"/>
       <c r="CT1" s="1"/>
@@ -10571,8 +10496,9 @@
       <c r="FO1" s="1"/>
       <c r="FP1" s="1"/>
       <c r="FQ1" s="1"/>
+      <c r="FR1" s="1"/>
     </row>
-    <row r="2" spans="1:182" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:183" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -10595,36 +10521,38 @@
         <v>9</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="L2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="M2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="N2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="P2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="Q2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="R2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="8"/>
       <c r="S2" s="8"/>
       <c r="T2" s="8"/>
       <c r="U2" s="8"/>
@@ -10700,8 +10628,8 @@
       <c r="CM2" s="8"/>
       <c r="CN2" s="8"/>
       <c r="CO2" s="8"/>
-      <c r="CP2" s="17"/>
-      <c r="CQ2" s="8"/>
+      <c r="CP2" s="8"/>
+      <c r="CQ2" s="17"/>
       <c r="CR2" s="8"/>
       <c r="CS2" s="8"/>
       <c r="CT2" s="8"/>
@@ -10789,10 +10717,11 @@
       <c r="FX2" s="8"/>
       <c r="FY2" s="8"/>
       <c r="FZ2" s="8"/>
+      <c r="GA2" s="8"/>
     </row>
-    <row r="3" spans="1:182" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:183" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>27</v>
@@ -10810,186 +10739,112 @@
       <c r="G3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>38</v>
+      <c r="H3" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>129</v>
+        <v>14</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>128</v>
+        <v>24</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Q3" s="14" t="s">
-        <v>128</v>
+        <v>50</v>
       </c>
       <c r="R3" s="14" t="s">
         <v>47</v>
       </c>
       <c r="S3" s="14" t="s">
-        <v>128</v>
+        <v>26</v>
       </c>
       <c r="T3" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U3" s="14" t="s">
-        <v>128</v>
+        <v>33</v>
       </c>
       <c r="V3" s="14" t="s">
-        <v>127</v>
+        <v>46</v>
       </c>
       <c r="W3" s="14" t="s">
-        <v>128</v>
+        <v>28</v>
       </c>
       <c r="X3" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Y3" s="14" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="Z3" s="14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AA3" s="14" t="s">
-        <v>128</v>
+        <v>30</v>
       </c>
       <c r="AB3" s="14" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="AC3" s="14" t="s">
-        <v>128</v>
+        <v>31</v>
       </c>
       <c r="AD3" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AF3" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AH3" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AJ3" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AK3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AL3" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="AM3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AN3" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="AO3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AP3" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="AQ3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AR3" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AT3" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="AU3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AV3" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="AW3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AX3" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="AY3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AZ3" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="BA3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="BB3" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="BC3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="BD3" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="BE3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="BF3" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="BG3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="BH3" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="BI3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="BJ3" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="BK3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="BL3" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="BM3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="BN3" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="BO3" s="14" t="s">
-        <v>128</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AE3" s="14"/>
+      <c r="AF3" s="14"/>
+      <c r="AG3" s="14"/>
+      <c r="AH3" s="14"/>
+      <c r="AI3" s="14"/>
+      <c r="AJ3" s="14"/>
+      <c r="AK3" s="14"/>
+      <c r="AL3" s="14"/>
+      <c r="AM3" s="14"/>
+      <c r="AN3" s="14"/>
+      <c r="AO3" s="14"/>
+      <c r="AP3" s="14"/>
+      <c r="AQ3" s="14"/>
+      <c r="AR3" s="14"/>
+      <c r="AS3" s="14"/>
+      <c r="AT3" s="14"/>
+      <c r="AU3" s="14"/>
+      <c r="AV3" s="14"/>
+      <c r="AW3" s="14"/>
+      <c r="AX3" s="14"/>
+      <c r="AY3" s="14"/>
+      <c r="AZ3" s="14"/>
+      <c r="BA3" s="14"/>
+      <c r="BB3" s="14"/>
+      <c r="BC3" s="14"/>
+      <c r="BD3" s="14"/>
+      <c r="BE3" s="14"/>
+      <c r="BF3" s="14"/>
+      <c r="BG3" s="14"/>
+      <c r="BH3" s="14"/>
+      <c r="BI3" s="14"/>
+      <c r="BJ3" s="14"/>
+      <c r="BK3" s="14"/>
+      <c r="BL3" s="14"/>
+      <c r="BM3" s="14"/>
+      <c r="BN3" s="14"/>
+      <c r="BO3" s="14"/>
       <c r="BP3" s="14"/>
       <c r="BQ3" s="14"/>
       <c r="BR3" s="14"/>
@@ -11016,10 +10871,11 @@
       <c r="CM3" s="14"/>
       <c r="CN3" s="14"/>
       <c r="CO3" s="14"/>
+      <c r="CP3" s="14"/>
     </row>
-    <row r="4" spans="1:182" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:183" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>27</v>
@@ -11037,45 +10893,99 @@
       <c r="G4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>67</v>
+      <c r="H4" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>129</v>
+        <v>15</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="14"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="14"/>
-      <c r="AB4" s="14"/>
-      <c r="AC4" s="14"/>
-      <c r="AD4" s="14"/>
-      <c r="AE4" s="14"/>
-      <c r="AF4" s="14"/>
-      <c r="AG4" s="14"/>
-      <c r="AH4" s="14"/>
-      <c r="AI4" s="14"/>
-      <c r="AJ4" s="14"/>
-      <c r="AK4" s="14"/>
-      <c r="AL4" s="14"/>
+        <v>40</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="S4" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="U4" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="V4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="W4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="X4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y4" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA4" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC4" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE4" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG4" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL4" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="AM4" s="14"/>
       <c r="AN4" s="14"/>
       <c r="AO4" s="14"/>
@@ -11131,10 +11041,11 @@
       <c r="CM4" s="14"/>
       <c r="CN4" s="14"/>
       <c r="CO4" s="14"/>
+      <c r="CP4" s="14"/>
     </row>
-    <row r="5" spans="1:182" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:183" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>27</v>
@@ -11152,90 +11063,84 @@
       <c r="G5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="3" t="s">
         <v>68</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>129</v>
+        <v>16</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>115</v>
+        <v>47</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>128</v>
+        <v>34</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>116</v>
+        <v>46</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>128</v>
+        <v>35</v>
       </c>
       <c r="N5" s="14" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>128</v>
+        <v>36</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>117</v>
+        <v>46</v>
       </c>
       <c r="Q5" s="14" t="s">
-        <v>128</v>
+        <v>37</v>
       </c>
       <c r="R5" s="14" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="S5" s="14" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="T5" s="14" t="s">
-        <v>118</v>
+        <v>46</v>
       </c>
       <c r="U5" s="14" t="s">
-        <v>128</v>
+        <v>39</v>
       </c>
       <c r="V5" s="14" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="W5" s="14" t="s">
-        <v>128</v>
+        <v>33</v>
       </c>
       <c r="X5" s="14" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="Y5" s="14" t="s">
-        <v>128</v>
+        <v>28</v>
       </c>
       <c r="Z5" s="14" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="AA5" s="14" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="AB5" s="14" t="s">
-        <v>119</v>
+        <v>46</v>
       </c>
       <c r="AC5" s="14" t="s">
-        <v>128</v>
+        <v>30</v>
       </c>
       <c r="AD5" s="14" t="s">
-        <v>120</v>
+        <v>46</v>
       </c>
       <c r="AE5" s="14" t="s">
-        <v>128</v>
+        <v>31</v>
       </c>
       <c r="AF5" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="AG5" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AH5" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="AI5" s="14" t="s">
-        <v>128</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AG5" s="14"/>
+      <c r="AH5" s="14"/>
+      <c r="AI5" s="14"/>
       <c r="AJ5" s="14"/>
       <c r="AK5" s="14"/>
       <c r="AL5" s="14"/>
@@ -11294,786 +11199,356 @@
       <c r="CM5" s="14"/>
       <c r="CN5" s="14"/>
       <c r="CO5" s="14"/>
-    </row>
-    <row r="6" spans="1:182" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="P6" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="R6" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="S6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="T6" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="U6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="V6" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="W6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="X6" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="Z6" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AB6" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AD6" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="AE6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AF6" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="AG6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AH6" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="AI6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AJ6" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="AK6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AL6" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="AM6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AN6" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="AO6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AP6" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="AQ6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AR6" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="AS6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AT6" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="AU6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AV6" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="AW6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AX6" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="AY6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AZ6" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="BA6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="BB6" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="BC6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="BD6" s="14"/>
-      <c r="BE6" s="14"/>
-      <c r="BF6" s="14"/>
-      <c r="BG6" s="14"/>
-      <c r="BH6" s="14"/>
-      <c r="BI6" s="14"/>
-      <c r="BJ6" s="14"/>
-      <c r="BK6" s="14"/>
-      <c r="BL6" s="14"/>
-      <c r="BM6" s="14"/>
-      <c r="BN6" s="14"/>
-      <c r="BO6" s="14"/>
-      <c r="BP6" s="14"/>
-      <c r="BQ6" s="14"/>
-      <c r="BR6" s="14"/>
-      <c r="BS6" s="14"/>
-      <c r="BT6" s="14"/>
-      <c r="BU6" s="14"/>
-      <c r="BV6" s="14"/>
-      <c r="BW6" s="14"/>
-      <c r="BX6" s="14"/>
-      <c r="BY6" s="14"/>
-      <c r="BZ6" s="14"/>
-      <c r="CA6" s="14"/>
-      <c r="CB6" s="14"/>
-      <c r="CC6" s="14"/>
-      <c r="CD6" s="14"/>
-      <c r="CE6" s="14"/>
-      <c r="CF6" s="14"/>
-      <c r="CG6" s="14"/>
-      <c r="CH6" s="14"/>
-      <c r="CI6" s="14"/>
-      <c r="CJ6" s="14"/>
-      <c r="CK6" s="14"/>
-      <c r="CL6" s="14"/>
-      <c r="CM6" s="14"/>
-      <c r="CN6" s="14"/>
-      <c r="CO6" s="14"/>
-    </row>
-    <row r="7" spans="1:182" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="14"/>
-      <c r="W7" s="14"/>
-      <c r="X7" s="14"/>
-      <c r="Y7" s="14"/>
-      <c r="Z7" s="14"/>
-      <c r="AA7" s="14"/>
-      <c r="AB7" s="14"/>
-      <c r="AC7" s="14"/>
-      <c r="AD7" s="14"/>
-      <c r="AE7" s="14"/>
-      <c r="AF7" s="14"/>
-      <c r="AG7" s="14"/>
-      <c r="AH7" s="14"/>
-      <c r="AI7" s="14"/>
-      <c r="AJ7" s="14"/>
-      <c r="AK7" s="14"/>
-      <c r="AL7" s="14"/>
-      <c r="AM7" s="14"/>
-      <c r="AN7" s="14"/>
-      <c r="AO7" s="14"/>
-      <c r="AP7" s="14"/>
-      <c r="AQ7" s="14"/>
-      <c r="AR7" s="14"/>
-      <c r="AS7" s="14"/>
-      <c r="AT7" s="14"/>
-      <c r="AU7" s="14"/>
-      <c r="AV7" s="14"/>
-      <c r="AW7" s="14"/>
-      <c r="AX7" s="14"/>
-      <c r="AY7" s="14"/>
-      <c r="AZ7" s="14"/>
-      <c r="BA7" s="14"/>
-      <c r="BB7" s="14"/>
-      <c r="BC7" s="14"/>
-      <c r="BD7" s="14"/>
-      <c r="BE7" s="14"/>
-      <c r="BF7" s="14"/>
-      <c r="BG7" s="14"/>
-      <c r="BH7" s="14"/>
-      <c r="BI7" s="14"/>
-      <c r="BJ7" s="14"/>
-      <c r="BK7" s="14"/>
-      <c r="BL7" s="14"/>
-      <c r="BM7" s="14"/>
-      <c r="BN7" s="14"/>
-      <c r="BO7" s="14"/>
-      <c r="BP7" s="14"/>
-      <c r="BQ7" s="14"/>
-      <c r="BR7" s="14"/>
-      <c r="BS7" s="14"/>
-      <c r="BT7" s="14"/>
-      <c r="BU7" s="14"/>
-      <c r="BV7" s="14"/>
-      <c r="BW7" s="14"/>
-      <c r="BX7" s="14"/>
-      <c r="BY7" s="14"/>
-      <c r="BZ7" s="14"/>
-      <c r="CA7" s="14"/>
-      <c r="CB7" s="14"/>
-      <c r="CC7" s="14"/>
-      <c r="CD7" s="14"/>
-      <c r="CE7" s="14"/>
-      <c r="CF7" s="14"/>
-      <c r="CG7" s="14"/>
-      <c r="CH7" s="14"/>
-      <c r="CI7" s="14"/>
-      <c r="CJ7" s="14"/>
-      <c r="CK7" s="14"/>
-      <c r="CL7" s="14"/>
-      <c r="CM7" s="14"/>
-      <c r="CN7" s="14"/>
-      <c r="CO7" s="14"/>
-    </row>
-    <row r="8" spans="1:182" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="K8" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="L8" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="M8" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="N8" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="O8" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="14"/>
-      <c r="Z8" s="14"/>
-      <c r="AA8" s="14"/>
-      <c r="AB8" s="14"/>
-      <c r="AC8" s="14"/>
-      <c r="AD8" s="14"/>
-      <c r="AE8" s="14"/>
-      <c r="AF8" s="14"/>
-      <c r="AG8" s="14"/>
-      <c r="AH8" s="14"/>
-      <c r="AI8" s="14"/>
-      <c r="AJ8" s="14"/>
-      <c r="AK8" s="14"/>
-      <c r="AL8" s="14"/>
-      <c r="AM8" s="14"/>
-      <c r="AN8" s="14"/>
-      <c r="AO8" s="14"/>
-      <c r="AP8" s="14"/>
-      <c r="AQ8" s="14"/>
-      <c r="AR8" s="14"/>
-      <c r="AS8" s="14"/>
-      <c r="AT8" s="14"/>
-      <c r="AU8" s="14"/>
-      <c r="AV8" s="14"/>
-      <c r="AW8" s="14"/>
-      <c r="AX8" s="14"/>
-      <c r="AY8" s="14"/>
-      <c r="AZ8" s="14"/>
-      <c r="BA8" s="14"/>
-      <c r="BB8" s="14"/>
-      <c r="BC8" s="14"/>
-      <c r="BD8" s="14"/>
-      <c r="BE8" s="14"/>
-      <c r="BF8" s="14"/>
-      <c r="BG8" s="14"/>
-      <c r="BH8" s="14"/>
-      <c r="BI8" s="14"/>
-      <c r="BJ8" s="14"/>
-      <c r="BK8" s="14"/>
-      <c r="BL8" s="14"/>
-      <c r="BM8" s="14"/>
-      <c r="BN8" s="14"/>
-      <c r="BO8" s="14"/>
-      <c r="BP8" s="14"/>
-      <c r="BQ8" s="14"/>
-      <c r="BR8" s="14"/>
-      <c r="BS8" s="14"/>
-      <c r="BT8" s="14"/>
-      <c r="BU8" s="14"/>
-      <c r="BV8" s="14"/>
-      <c r="BW8" s="14"/>
-      <c r="BX8" s="14"/>
-      <c r="BY8" s="14"/>
-      <c r="BZ8" s="14"/>
-      <c r="CA8" s="14"/>
-      <c r="CB8" s="14"/>
-      <c r="CC8" s="14"/>
-      <c r="CD8" s="14"/>
-      <c r="CE8" s="14"/>
-      <c r="CF8" s="14"/>
-      <c r="CG8" s="14"/>
-      <c r="CH8" s="14"/>
-      <c r="CI8" s="14"/>
-      <c r="CJ8" s="14"/>
-      <c r="CK8" s="14"/>
-      <c r="CL8" s="14"/>
-      <c r="CM8" s="14"/>
-      <c r="CN8" s="14"/>
-      <c r="CO8" s="14"/>
-    </row>
-    <row r="9" spans="1:182" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="N9" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="O9" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="P9" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q9" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="R9" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="S9" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="T9" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="U9" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="V9" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="W9" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="X9" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y9" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="Z9" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA9" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AB9" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC9" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AD9" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE9" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AF9" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="AG9" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AH9" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI9" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AJ9" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK9" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AL9" s="14"/>
-      <c r="AM9" s="14"/>
-      <c r="AN9" s="14"/>
-      <c r="AO9" s="14"/>
-      <c r="AP9" s="14"/>
-      <c r="AQ9" s="14"/>
-      <c r="AR9" s="14"/>
-      <c r="AS9" s="14"/>
-      <c r="AT9" s="14"/>
-      <c r="AU9" s="14"/>
-      <c r="AV9" s="14"/>
-      <c r="AW9" s="14"/>
-      <c r="AX9" s="14"/>
-      <c r="AY9" s="14"/>
-      <c r="AZ9" s="14"/>
-      <c r="BA9" s="14"/>
-      <c r="BB9" s="14"/>
-      <c r="BC9" s="14"/>
-      <c r="BD9" s="14"/>
-      <c r="BE9" s="14"/>
-      <c r="BF9" s="14"/>
-      <c r="BG9" s="14"/>
-      <c r="BH9" s="14"/>
-      <c r="BI9" s="14"/>
-      <c r="BJ9" s="14"/>
-      <c r="BK9" s="14"/>
-      <c r="BL9" s="14"/>
-      <c r="BM9" s="14"/>
-      <c r="BN9" s="14"/>
-      <c r="BO9" s="14"/>
-      <c r="BP9" s="14"/>
-      <c r="BQ9" s="14"/>
-      <c r="BR9" s="14"/>
-      <c r="BS9" s="14"/>
-      <c r="BT9" s="14"/>
-      <c r="BU9" s="14"/>
-      <c r="BV9" s="14"/>
-      <c r="BW9" s="14"/>
-      <c r="BX9" s="14"/>
-      <c r="BY9" s="14"/>
-      <c r="BZ9" s="14"/>
-      <c r="CA9" s="14"/>
-      <c r="CB9" s="14"/>
-      <c r="CC9" s="14"/>
-      <c r="CD9" s="14"/>
-      <c r="CE9" s="14"/>
-      <c r="CF9" s="14"/>
-      <c r="CG9" s="14"/>
-      <c r="CH9" s="14"/>
-      <c r="CI9" s="14"/>
-      <c r="CJ9" s="14"/>
-      <c r="CK9" s="14"/>
-      <c r="CL9" s="14"/>
-      <c r="CM9" s="14"/>
-      <c r="CN9" s="14"/>
-      <c r="CO9" s="14"/>
-    </row>
-    <row r="10" spans="1:182" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="K10" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="L10" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="M10" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="N10" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="O10" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="P10" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q10" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="R10" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="S10" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="T10" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="U10" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="V10" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="W10" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="X10" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y10" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="Z10" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA10" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AB10" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC10" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AD10" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE10" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AF10" s="14"/>
-      <c r="AG10" s="14"/>
-      <c r="AH10" s="14"/>
-      <c r="AI10" s="14"/>
-      <c r="AJ10" s="14"/>
-      <c r="AK10" s="14"/>
-      <c r="AL10" s="14"/>
-      <c r="AM10" s="14"/>
-      <c r="AN10" s="14"/>
-      <c r="AO10" s="14"/>
-      <c r="AP10" s="14"/>
-      <c r="AQ10" s="14"/>
-      <c r="AR10" s="14"/>
-      <c r="AS10" s="14"/>
-      <c r="AT10" s="14"/>
-      <c r="AU10" s="14"/>
-      <c r="AV10" s="14"/>
-      <c r="AW10" s="14"/>
-      <c r="AX10" s="14"/>
-      <c r="AY10" s="14"/>
-      <c r="AZ10" s="14"/>
-      <c r="BA10" s="14"/>
-      <c r="BB10" s="14"/>
-      <c r="BC10" s="14"/>
-      <c r="BD10" s="14"/>
-      <c r="BE10" s="14"/>
-      <c r="BF10" s="14"/>
-      <c r="BG10" s="14"/>
-      <c r="BH10" s="14"/>
-      <c r="BI10" s="14"/>
-      <c r="BJ10" s="14"/>
-      <c r="BK10" s="14"/>
-      <c r="BL10" s="14"/>
-      <c r="BM10" s="14"/>
-      <c r="BN10" s="14"/>
-      <c r="BO10" s="14"/>
-      <c r="BP10" s="14"/>
-      <c r="BQ10" s="14"/>
-      <c r="BR10" s="14"/>
-      <c r="BS10" s="14"/>
-      <c r="BT10" s="14"/>
-      <c r="BU10" s="14"/>
-      <c r="BV10" s="14"/>
-      <c r="BW10" s="14"/>
-      <c r="BX10" s="14"/>
-      <c r="BY10" s="14"/>
-      <c r="BZ10" s="14"/>
-      <c r="CA10" s="14"/>
-      <c r="CB10" s="14"/>
-      <c r="CC10" s="14"/>
-      <c r="CD10" s="14"/>
-      <c r="CE10" s="14"/>
-      <c r="CF10" s="14"/>
-      <c r="CG10" s="14"/>
-      <c r="CH10" s="14"/>
-      <c r="CI10" s="14"/>
-      <c r="CJ10" s="14"/>
-      <c r="CK10" s="14"/>
-      <c r="CL10" s="14"/>
-      <c r="CM10" s="14"/>
-      <c r="CN10" s="14"/>
-      <c r="CO10" s="14"/>
+      <c r="CP5" s="14"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BO3 BQ3 AE5:AE6 AO3 AQ3 AS3 AU3 AW3 AY3 BA3 BC3 BE3 BE6 BI3 BK3 BM3 BG3 AG9 AI9 AK9 AG5:AG6 AI5:AI6 AK5:AK6 AM6 AO6 AQ6 AS6 AU6 AW6 AY6 BA6 BC6 AE9:AE10 I3:I10 AG3 AC3:AC10 K3:K10 O3:O10 AK3 AM3 AI3 S3:S10 Q3:Q10 M3:M10 Y3:Y10 AA3:AA10 W3:W10 AE3 U3:U10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF3 AN3 AP3 AR3 AT3 AV3 AX3 AZ3 BB3 BD3 J3:J5 Z3:Z5 L3:L5 P3:P5 T3:T5 R3:R5 N3:N5 AB3:AB5 X3:X5 V3:V5 AH3:AH4 AF3:AF5 AL3:AL4 AJ3:AJ4 AD3:AD5">
       <formula1>"Not Started,In Progress,Implemented"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="E6" r:id="rId4"/>
-    <hyperlink ref="E7" r:id="rId5"/>
-    <hyperlink ref="E8" r:id="rId6"/>
+    <hyperlink ref="E3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="73.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.85546875" customWidth="1"/>
+    <col min="13" max="13" width="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" customWidth="1"/>
+    <col min="16" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="21">
+        <v>9</v>
+      </c>
+      <c r="K1" s="21">
+        <v>10</v>
+      </c>
+      <c r="L1" s="21">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1">
+        <v>12</v>
+      </c>
+      <c r="N1" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="26"/>
+    </row>
+    <row r="2" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="14" t="str">
+        <f>'Configure Offerings'!H3</f>
+        <v>DevOps v0_001</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="O3" s="3">
+        <v>5</v>
+      </c>
+      <c r="P3" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q3" s="22">
+        <v>1027428</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="N1:S1"/>
+  </mergeCells>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3">
+      <formula1>OFFSET(INDIRECT(SUBSTITUTE(I3," ","")),0,0,COUNTA(INDIRECT(SUBSTITUTE(I3," ","")&amp;"Col")),1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3">
+      <formula1>INDIRECT(SUBSTITUTE(I3&amp;J3&amp;K3," ",""))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3">
+      <formula1>MainTaskFolder</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3">
+      <formula1>OFFSET(INDIRECT(SUBSTITUTE(I3&amp;J3," ","")),0,0,COUNTA(INDIRECT(SUBSTITUTE(I3&amp;J3," ","")&amp;"Col")),1)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3 R3">
+      <formula1>N3</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FU3"/>
   <sheetViews>
@@ -12943,11 +12418,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FU3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>

</xml_diff>